<commit_message>
Update shooter calibration data for Kentwood.
</commit_message>
<xml_diff>
--- a/conf/shooter_data.xlsx
+++ b/conf/shooter_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -369,18 +369,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D71" sqref="D71"/>
+      <selection pane="bottomRight" sqref="A1:E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -397,834 +397,834 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>1317.172</v>
+        <v>1428.02</v>
       </c>
       <c r="D2" s="2">
-        <v>439.9076</v>
+        <v>437.23645671509507</v>
       </c>
       <c r="E2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="2">
-        <v>1335.9460000000001</v>
+        <v>1446.877</v>
       </c>
       <c r="D3" s="2">
-        <v>441.00120000000004</v>
+        <v>437.93711585281255</v>
       </c>
       <c r="E3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>1354.72</v>
+        <v>1465.7339999999999</v>
       </c>
       <c r="D4" s="2">
-        <v>442.09480000000002</v>
+        <v>438.6909663204865</v>
       </c>
       <c r="E4">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" s="2">
-        <v>1373.4939999999999</v>
+        <v>1484.5909999999999</v>
       </c>
       <c r="D5" s="2">
-        <v>443.1884</v>
+        <v>439.49522807209462</v>
       </c>
       <c r="E5">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" s="2">
-        <v>1392.268</v>
+        <v>1503.4480000000001</v>
       </c>
       <c r="D6" s="2">
-        <v>444.28200000000004</v>
+        <v>440.34717763552874</v>
       </c>
       <c r="E6">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>1411.0420000000001</v>
+        <v>1522.3050000000001</v>
       </c>
       <c r="D7" s="2">
-        <v>445.37560000000002</v>
+        <v>441.24414811259408</v>
       </c>
       <c r="E7">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" s="2">
-        <v>1429.816</v>
+        <v>1541.162</v>
       </c>
       <c r="D8" s="2">
-        <v>446.4692</v>
+        <v>442.18352917901086</v>
       </c>
       <c r="E8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" s="2">
-        <v>1448.59</v>
+        <v>1560.019</v>
       </c>
       <c r="D9" s="2">
-        <v>447.56280000000004</v>
+        <v>443.16276708441217</v>
       </c>
       <c r="E9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" s="2">
-        <v>1467.364</v>
+        <v>1578.876</v>
       </c>
       <c r="D10" s="2">
-        <v>448.65640000000002</v>
+        <v>444.17936465234629</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" s="2">
-        <v>1486.1380000000001</v>
+        <v>1597.7329999999999</v>
       </c>
       <c r="D11" s="2">
-        <v>449.75</v>
+        <v>445.23088128027496</v>
       </c>
       <c r="E11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" s="2">
-        <v>1504.912</v>
+        <v>1616.59</v>
       </c>
       <c r="D12" s="2">
-        <v>450.84360000000004</v>
+        <v>446.31493293957374</v>
       </c>
       <c r="E12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13" s="2">
-        <v>1523.6859999999999</v>
+        <v>1635.4469999999999</v>
       </c>
       <c r="D13" s="2">
-        <v>451.93720000000002</v>
+        <v>447.4291921755331</v>
       </c>
       <c r="E13">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14" s="2">
-        <v>1542.46</v>
+        <v>1654.3039999999999</v>
       </c>
       <c r="D14" s="2">
-        <v>453.0308</v>
+        <v>448.57138810735626</v>
       </c>
       <c r="E14">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15" s="2">
-        <v>1561.2340000000002</v>
+        <v>1673.1610000000001</v>
       </c>
       <c r="D15" s="2">
-        <v>454.12440000000004</v>
+        <v>449.73930642816163</v>
       </c>
       <c r="E15">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16" s="2">
-        <v>1580.008</v>
+        <v>1692.018</v>
       </c>
       <c r="D16" s="2">
-        <v>455.21800000000002</v>
+        <v>450.93078940498094</v>
       </c>
       <c r="E16">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17" s="2">
-        <v>1598.7819999999999</v>
+        <v>1710.875</v>
       </c>
       <c r="D17" s="2">
-        <v>456.3116</v>
+        <v>452.14373587876048</v>
       </c>
       <c r="E17">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18" s="2">
-        <v>1617.556</v>
+        <v>1729.732</v>
       </c>
       <c r="D18" s="2">
-        <v>457.40520000000004</v>
+        <v>453.37610126436027</v>
       </c>
       <c r="E18">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19" s="2">
-        <v>1636.3300000000002</v>
+        <v>1748.5889999999999</v>
       </c>
       <c r="D19" s="2">
-        <v>458.49880000000002</v>
+        <v>454.62589755055444</v>
       </c>
       <c r="E19">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20" s="2">
-        <v>1655.104</v>
+        <v>1767.4459999999999</v>
       </c>
       <c r="D20" s="2">
-        <v>459.5924</v>
+        <v>455.89119330003086</v>
       </c>
       <c r="E20">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" s="2">
-        <v>1673.8779999999999</v>
+        <v>1786.3029999999999</v>
       </c>
       <c r="D21" s="2">
-        <v>460.68600000000004</v>
+        <v>457.17011364939196</v>
       </c>
       <c r="E21">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22" s="2">
-        <v>1692.652</v>
+        <v>1805.16</v>
       </c>
       <c r="D22" s="2">
-        <v>461.77960000000002</v>
+        <v>458.46084030915415</v>
       </c>
       <c r="E22">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23" s="2">
-        <v>1711.4260000000002</v>
+        <v>1824.0170000000001</v>
       </c>
       <c r="D23" s="2">
-        <v>462.8732</v>
+        <v>459.76161156374712</v>
       </c>
       <c r="E23">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24" s="2">
-        <v>1730.2</v>
+        <v>1842.874</v>
       </c>
       <c r="D24" s="2">
-        <v>463.96680000000003</v>
+        <v>461.07072227151582</v>
       </c>
       <c r="E24">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25" s="2">
-        <v>1748.9739999999999</v>
+        <v>1861.731</v>
       </c>
       <c r="D25" s="2">
-        <v>465.06040000000002</v>
+        <v>462.38652386471847</v>
       </c>
       <c r="E25">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26" s="2">
-        <v>1767.748</v>
+        <v>1880.588</v>
       </c>
       <c r="D26" s="2">
-        <v>466.154</v>
+        <v>463.70742434952706</v>
       </c>
       <c r="E26">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27" s="2">
-        <v>1786.5220000000002</v>
+        <v>1899.4449999999999</v>
       </c>
       <c r="D27" s="2">
-        <v>467.24760000000003</v>
+        <v>465.03188830602869</v>
       </c>
       <c r="E27">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28" s="2">
-        <v>1805.296</v>
+        <v>1918.3019999999999</v>
       </c>
       <c r="D28" s="2">
-        <v>468.34120000000001</v>
+        <v>466.35843688822308</v>
       </c>
       <c r="E28">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29" s="2">
-        <v>1824.07</v>
+        <v>1937.1589999999999</v>
       </c>
       <c r="D29" s="2">
-        <v>469.4348</v>
+        <v>467.6856478240253</v>
       </c>
       <c r="E29">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30" s="2">
-        <v>1842.8440000000001</v>
+        <v>1956.0159999999998</v>
       </c>
       <c r="D30" s="2">
-        <v>470.52840000000003</v>
+        <v>469.01215541526369</v>
       </c>
       <c r="E30">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31" s="2">
-        <v>1861.6180000000002</v>
+        <v>1974.873</v>
       </c>
       <c r="D31" s="2">
-        <v>471.62200000000001</v>
+        <v>470.33665053768084</v>
       </c>
       <c r="E31">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32" s="2">
-        <v>1880.3920000000001</v>
+        <v>1993.73</v>
       </c>
       <c r="D32" s="2">
-        <v>472.71559999999999</v>
+        <v>471.65788064093329</v>
       </c>
       <c r="E32">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33" s="2">
-        <v>1899.1659999999999</v>
+        <v>2012.587</v>
       </c>
       <c r="D33" s="2">
-        <v>473.80920000000003</v>
+        <v>472.97464974859179</v>
       </c>
       <c r="E33">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34" s="2">
-        <v>1917.94</v>
+        <v>2031.444</v>
       </c>
       <c r="D34" s="2">
-        <v>474.90280000000001</v>
+        <v>474.28581845814108</v>
       </c>
       <c r="E34">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35" s="2">
-        <v>1936.7140000000002</v>
+        <v>2050.3009999999999</v>
       </c>
       <c r="D35" s="2">
-        <v>475.99639999999999</v>
+        <v>475.59030394098011</v>
       </c>
       <c r="E35">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
       <c r="C36" s="2">
-        <v>1955.4880000000001</v>
+        <v>2069.1579999999999</v>
       </c>
       <c r="D36" s="2">
-        <v>477.09000000000003</v>
+        <v>476.88707994242088</v>
       </c>
       <c r="E36">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37" s="2">
-        <v>1974.2619999999999</v>
+        <v>2088.0149999999999</v>
       </c>
       <c r="D37" s="2">
-        <v>478.18360000000001</v>
+        <v>478.17517678169077</v>
       </c>
       <c r="E37">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="C38" s="2">
-        <v>1993.0360000000001</v>
+        <v>2106.8719999999998</v>
       </c>
       <c r="D38" s="2">
-        <v>479.27719999999999</v>
+        <v>479.45368135193064</v>
       </c>
       <c r="E38">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="C39" s="2">
-        <v>2011.8100000000002</v>
+        <v>2125.7289999999998</v>
       </c>
       <c r="D39" s="2">
-        <v>480.37080000000003</v>
+        <v>480.7217371201956</v>
       </c>
       <c r="E39">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
       <c r="C40" s="2">
-        <v>2030.5840000000001</v>
+        <v>2144.5859999999998</v>
       </c>
       <c r="D40" s="2">
-        <v>481.46440000000001</v>
+        <v>481.97854412745403</v>
       </c>
       <c r="E40">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41" s="2">
-        <v>2049.3580000000002</v>
+        <v>2163.4429999999998</v>
       </c>
       <c r="D41" s="2">
-        <v>482.55799999999999</v>
+        <v>483.22335898858944</v>
       </c>
       <c r="E41">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42" s="2">
-        <v>2068.1320000000001</v>
+        <v>2182.2999999999997</v>
       </c>
       <c r="D42" s="2">
-        <v>483.65160000000003</v>
+        <v>484.45549489239863</v>
       </c>
       <c r="E42">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43" s="2">
-        <v>2086.9060000000004</v>
+        <v>2201.1569999999997</v>
       </c>
       <c r="D43" s="2">
-        <v>484.74520000000001</v>
+        <v>485.67432160159194</v>
       </c>
       <c r="E43">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44" s="2">
-        <v>2105.6800000000003</v>
+        <v>2220.0139999999997</v>
       </c>
       <c r="D44" s="2">
-        <v>485.83879999999999</v>
+        <v>486.87926545279595</v>
       </c>
       <c r="E44">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45" s="2">
-        <v>2124.4540000000002</v>
+        <v>2238.8709999999996</v>
       </c>
       <c r="D45" s="2">
-        <v>486.93240000000003</v>
+        <v>488.06980935654826</v>
       </c>
       <c r="E45">
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46" s="2">
-        <v>2143.2280000000005</v>
+        <v>2257.7279999999996</v>
       </c>
       <c r="D46" s="2">
-        <v>488.02600000000001</v>
+        <v>489.24549279730365</v>
       </c>
       <c r="E46">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47" s="2">
-        <v>2162.0020000000004</v>
+        <v>2276.5849999999996</v>
       </c>
       <c r="D47" s="2">
-        <v>489.11959999999999</v>
+        <v>490.40591183342792</v>
       </c>
       <c r="E47">
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48" s="2">
-        <v>2180.7760000000003</v>
+        <v>2295.4419999999996</v>
       </c>
       <c r="D48" s="2">
-        <v>490.21320000000003</v>
+        <v>491.55071909720243</v>
       </c>
       <c r="E48">
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="C49" s="2">
-        <v>2199.5500000000002</v>
+        <v>2314.2989999999995</v>
       </c>
       <c r="D49" s="2">
-        <v>491.30680000000001</v>
+        <v>492.67962379482344</v>
       </c>
       <c r="E49">
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50" s="2">
-        <v>2218.3240000000001</v>
+        <v>2333.1559999999999</v>
       </c>
       <c r="D50" s="2">
-        <v>492.40039999999999</v>
+        <v>493.79239170639937</v>
       </c>
       <c r="E50">
         <v>8</v>
@@ -1232,16 +1232,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51" s="2">
-        <v>2237.0980000000004</v>
+        <v>2352.0129999999999</v>
       </c>
       <c r="D51" s="2">
-        <v>493.49400000000003</v>
+        <v>494.88884518595376</v>
       </c>
       <c r="E51">
         <v>8</v>
@@ -1249,16 +1249,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52" s="2">
-        <v>2255.8720000000003</v>
+        <v>2370.87</v>
       </c>
       <c r="D52" s="2">
-        <v>494.58760000000001</v>
+        <v>495.96886316142434</v>
       </c>
       <c r="E52">
         <v>8</v>
@@ -1266,16 +1266,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53" s="2">
-        <v>2274.6460000000002</v>
+        <v>2389.7269999999999</v>
       </c>
       <c r="D53" s="2">
-        <v>495.68119999999999</v>
+        <v>497.03238113466193</v>
       </c>
       <c r="E53">
         <v>8</v>
@@ -1283,16 +1283,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="C54" s="2">
-        <v>2293.4200000000005</v>
+        <v>2408.5839999999998</v>
       </c>
       <c r="D54" s="2">
-        <v>496.77480000000003</v>
+        <v>498.07939118143315</v>
       </c>
       <c r="E54">
         <v>8</v>
@@ -1300,16 +1300,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55" s="2">
-        <v>2312.1940000000004</v>
+        <v>2427.4409999999998</v>
       </c>
       <c r="D55" s="2">
-        <v>497.86840000000001</v>
+        <v>499.10994195141632</v>
       </c>
       <c r="E55">
         <v>8</v>
@@ -1317,16 +1317,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="C56" s="2">
-        <v>2330.9680000000003</v>
+        <v>2446.2979999999998</v>
       </c>
       <c r="D56" s="2">
-        <v>498.96199999999999</v>
+        <v>500.12413866820577</v>
       </c>
       <c r="E56">
         <v>8</v>
@@ -1334,16 +1334,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B57">
         <v>0</v>
       </c>
       <c r="C57" s="2">
-        <v>2349.7420000000002</v>
+        <v>2465.1549999999997</v>
       </c>
       <c r="D57" s="2">
-        <v>500.05560000000003</v>
+        <v>501.12214312930848</v>
       </c>
       <c r="E57">
         <v>8</v>
@@ -1351,16 +1351,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
       <c r="C58" s="2">
-        <v>2368.5160000000001</v>
+        <v>2484.0119999999997</v>
       </c>
       <c r="D58" s="2">
-        <v>501.14920000000001</v>
+        <v>502.1041737061463</v>
       </c>
       <c r="E58">
         <v>8</v>
@@ -1368,16 +1368,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
       <c r="C59" s="2">
-        <v>2387.2900000000004</v>
+        <v>2502.8689999999997</v>
       </c>
       <c r="D59" s="2">
-        <v>502.24279999999999</v>
+        <v>503.07050534405528</v>
       </c>
       <c r="E59">
         <v>8</v>
@@ -1385,16 +1385,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
       <c r="C60" s="2">
-        <v>2406.0640000000003</v>
+        <v>2521.7259999999997</v>
       </c>
       <c r="D60" s="2">
-        <v>503.33640000000003</v>
+        <v>504.02146956228432</v>
       </c>
       <c r="E60">
         <v>8</v>
@@ -1402,16 +1402,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
       <c r="C61" s="2">
-        <v>2424.8380000000002</v>
+        <v>2540.5829999999996</v>
       </c>
       <c r="D61" s="2">
-        <v>504.43</v>
+        <v>504.95745445399837</v>
       </c>
       <c r="E61">
         <v>8</v>
@@ -1419,16 +1419,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
       <c r="C62" s="2">
-        <v>2443.6120000000005</v>
+        <v>2559.4399999999996</v>
       </c>
       <c r="D62" s="2">
-        <v>505.52359999999999</v>
+        <v>505.87890468627472</v>
       </c>
       <c r="E62">
         <v>8</v>
@@ -1436,16 +1436,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
       <c r="C63" s="2">
-        <v>2462.3860000000004</v>
+        <v>2578.2969999999996</v>
       </c>
       <c r="D63" s="2">
-        <v>506.61720000000003</v>
+        <v>506.78632150010424</v>
       </c>
       <c r="E63">
         <v>8</v>
@@ -1453,16 +1453,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B64">
         <v>0</v>
       </c>
       <c r="C64" s="2">
-        <v>2481.1600000000003</v>
+        <v>2597.1539999999995</v>
       </c>
       <c r="D64" s="2">
-        <v>507.71080000000001</v>
+        <v>507.68026271039378</v>
       </c>
       <c r="E64">
         <v>8</v>
@@ -1470,16 +1470,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
       <c r="C65" s="2">
-        <v>2499.9340000000002</v>
+        <v>2616.0109999999995</v>
       </c>
       <c r="D65" s="2">
-        <v>508.80439999999999</v>
+        <v>508.56134270596306</v>
       </c>
       <c r="E65">
         <v>8</v>
@@ -1487,16 +1487,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="C66" s="2">
-        <v>2518.7080000000001</v>
+        <v>2634.8679999999995</v>
       </c>
       <c r="D66" s="2">
-        <v>509.89800000000002</v>
+        <v>509.43023244954577</v>
       </c>
       <c r="E66">
         <v>8</v>
@@ -1504,16 +1504,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="C67" s="2">
-        <v>2537.4820000000004</v>
+        <v>2653.7249999999999</v>
       </c>
       <c r="D67" s="2">
-        <v>510.99160000000001</v>
+        <v>510.28765947779073</v>
       </c>
       <c r="E67">
         <v>8</v>
@@ -1521,16 +1521,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
       <c r="C68" s="2">
-        <v>2556.2560000000003</v>
+        <v>2672.5819999999999</v>
       </c>
       <c r="D68" s="2">
-        <v>512.08519999999999</v>
+        <v>511.1344079012589</v>
       </c>
       <c r="E68">
         <v>8</v>
@@ -1538,16 +1538,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="C69" s="2">
-        <v>2575.0300000000002</v>
+        <v>2691.4389999999999</v>
       </c>
       <c r="D69" s="2">
-        <v>513.17880000000002</v>
+        <v>511.97131840442705</v>
       </c>
       <c r="E69">
         <v>8</v>
@@ -1555,16 +1555,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="C70" s="2">
-        <v>2593.8040000000005</v>
+        <v>2710.2959999999998</v>
       </c>
       <c r="D70" s="2">
-        <v>514.27240000000006</v>
+        <v>512.79928824568435</v>
       </c>
       <c r="E70">
         <v>8</v>
@@ -1572,16 +1572,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
       <c r="C71" s="2">
-        <v>2612.5780000000004</v>
+        <v>2729.1529999999998</v>
       </c>
       <c r="D71" s="2">
-        <v>515.36599999999999</v>
+        <v>513.61927125733644</v>
       </c>
       <c r="E71">
         <v>8</v>
@@ -1589,16 +1589,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B72">
         <v>0</v>
       </c>
       <c r="C72" s="2">
-        <v>2631.3520000000003</v>
+        <v>2748.0099999999998</v>
       </c>
       <c r="D72" s="2">
-        <v>516.45960000000002</v>
+        <v>514.43227784559997</v>
       </c>
       <c r="E72">
         <v>8</v>
@@ -1606,16 +1606,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
       <c r="C73" s="2">
-        <v>2650.1260000000002</v>
+        <v>2766.8669999999997</v>
       </c>
       <c r="D73" s="2">
-        <v>517.55320000000006</v>
+        <v>515.23937499060901</v>
       </c>
       <c r="E73">
         <v>8</v>
@@ -1623,16 +1623,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B74">
         <v>0</v>
       </c>
       <c r="C74" s="2">
-        <v>2668.9</v>
+        <v>2785.7239999999997</v>
       </c>
       <c r="D74" s="2">
-        <v>518.64679999999998</v>
+        <v>516.04168624640681</v>
       </c>
       <c r="E74">
         <v>8</v>
@@ -1640,16 +1640,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B75">
         <v>0</v>
       </c>
       <c r="C75" s="2">
-        <v>2687.6740000000004</v>
+        <v>2804.5809999999997</v>
       </c>
       <c r="D75" s="2">
-        <v>519.74040000000002</v>
+        <v>516.84039174095608</v>
       </c>
       <c r="E75">
         <v>8</v>
@@ -1657,16 +1657,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B76">
         <v>0</v>
       </c>
       <c r="C76" s="2">
-        <v>2706.4480000000003</v>
+        <v>2823.4379999999996</v>
       </c>
       <c r="D76" s="2">
-        <v>520.83400000000006</v>
+        <v>517.6367281761319</v>
       </c>
       <c r="E76">
         <v>8</v>
@@ -1674,16 +1674,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
       <c r="C77" s="2">
-        <v>2725.2220000000002</v>
+        <v>2842.2949999999996</v>
       </c>
       <c r="D77" s="2">
-        <v>521.92759999999998</v>
+        <v>518.43198882772015</v>
       </c>
       <c r="E77">
         <v>8</v>
@@ -1691,16 +1691,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B78">
         <v>0</v>
       </c>
       <c r="C78" s="2">
-        <v>2743.9960000000005</v>
+        <v>2861.1519999999996</v>
       </c>
       <c r="D78" s="2">
-        <v>523.02120000000002</v>
+        <v>519.22752354542502</v>
       </c>
       <c r="E78">
         <v>8</v>
@@ -1708,16 +1708,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B79">
         <v>0</v>
       </c>
       <c r="C79" s="2">
-        <v>2762.7700000000004</v>
+        <v>2880.0089999999996</v>
       </c>
       <c r="D79" s="2">
-        <v>524.11480000000006</v>
+        <v>520.02473875286171</v>
       </c>
       <c r="E79">
         <v>8</v>
@@ -1725,16 +1725,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B80">
         <v>0</v>
       </c>
       <c r="C80" s="2">
-        <v>2781.5440000000003</v>
+        <v>2898.8659999999995</v>
       </c>
       <c r="D80" s="2">
-        <v>525.20839999999998</v>
+        <v>520.82509744756146</v>
       </c>
       <c r="E80">
         <v>8</v>
@@ -1742,16 +1742,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B81">
         <v>0</v>
       </c>
       <c r="C81" s="2">
-        <v>2800.3180000000002</v>
+        <v>2917.7229999999995</v>
       </c>
       <c r="D81" s="2">
-        <v>526.30200000000002</v>
+        <v>521.63011920096835</v>
       </c>
       <c r="E81">
         <v>8</v>
@@ -1759,16 +1759,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B82">
         <v>0</v>
       </c>
       <c r="C82" s="2">
-        <v>2819.0920000000001</v>
+        <v>2936.58</v>
       </c>
       <c r="D82" s="2">
-        <v>527.39560000000006</v>
+        <v>522.44138015844248</v>
       </c>
       <c r="E82">
         <v>8</v>
@@ -1776,16 +1776,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B83">
         <v>0</v>
       </c>
       <c r="C83" s="2">
-        <v>2837.8660000000004</v>
+        <v>2955.4369999999999</v>
       </c>
       <c r="D83" s="2">
-        <v>528.48919999999998</v>
+        <v>523.26051303925362</v>
       </c>
       <c r="E83">
         <v>8</v>
@@ -1793,16 +1793,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B84">
         <v>0</v>
       </c>
       <c r="C84" s="2">
-        <v>2856.6400000000003</v>
+        <v>2974.2939999999999</v>
       </c>
       <c r="D84" s="2">
-        <v>529.58280000000002</v>
+        <v>524.08920713659074</v>
       </c>
       <c r="E84">
         <v>8</v>
@@ -1810,16 +1810,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B85">
         <v>0</v>
       </c>
       <c r="C85" s="2">
-        <v>2875.4140000000002</v>
+        <v>2993.1509999999998</v>
       </c>
       <c r="D85" s="2">
-        <v>530.67640000000006</v>
+        <v>524.92920831755475</v>
       </c>
       <c r="E85">
         <v>8</v>
@@ -1827,18 +1827,426 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
       <c r="C86" s="2">
-        <v>2894.1880000000006</v>
+        <v>3012.0079999999998</v>
       </c>
       <c r="D86" s="2">
-        <v>531.77</v>
+        <v>525.78231902315804</v>
       </c>
       <c r="E86">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>157</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>3030.8649999999998</v>
+      </c>
+      <c r="D87">
+        <v>526.65039826833174</v>
+      </c>
+      <c r="E87">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>158</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>3049.7219999999998</v>
+      </c>
+      <c r="D88">
+        <v>527.53536164191667</v>
+      </c>
+      <c r="E88">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>159</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>3068.5789999999997</v>
+      </c>
+      <c r="D89">
+        <v>528.439181306671</v>
+      </c>
+      <c r="E89">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>160</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>3087.4359999999997</v>
+      </c>
+      <c r="D90">
+        <v>529.36388599926488</v>
+      </c>
+      <c r="E90">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>161</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>3106.2929999999997</v>
+      </c>
+      <c r="D91">
+        <v>530.31156103028582</v>
+      </c>
+      <c r="E91">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>162</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>3125.1499999999996</v>
+      </c>
+      <c r="D92">
+        <v>531.2843482842278</v>
+      </c>
+      <c r="E92">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>163</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>3144.0069999999996</v>
+      </c>
+      <c r="D93">
+        <v>532.28444621950769</v>
+      </c>
+      <c r="E93">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>164</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>3162.8639999999996</v>
+      </c>
+      <c r="D94">
+        <v>533.31410986845106</v>
+      </c>
+      <c r="E94">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>165</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>3181.7209999999995</v>
+      </c>
+      <c r="D95">
+        <v>534.3756508373009</v>
+      </c>
+      <c r="E95">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>166</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>3200.5779999999995</v>
+      </c>
+      <c r="D96">
+        <v>535.47143730620849</v>
+      </c>
+      <c r="E96">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>167</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>3219.4349999999995</v>
+      </c>
+      <c r="D97">
+        <v>536.60389402924659</v>
+      </c>
+      <c r="E97">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>168</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>3238.2919999999995</v>
+      </c>
+      <c r="D98">
+        <v>537.77550233439626</v>
+      </c>
+      <c r="E98">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>169</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>3257.1489999999999</v>
+      </c>
+      <c r="D99">
+        <v>538.98880012355596</v>
+      </c>
+      <c r="E99">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>170</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>3276.0059999999999</v>
+      </c>
+      <c r="D100">
+        <v>540.24638187253697</v>
+      </c>
+      <c r="E100">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>171</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>3294.8629999999998</v>
+      </c>
+      <c r="D101">
+        <v>541.55089863106252</v>
+      </c>
+      <c r="E101">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>172</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>3313.72</v>
+      </c>
+      <c r="D102">
+        <v>542.9050580227746</v>
+      </c>
+      <c r="E102">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>173</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>3332.5769999999998</v>
+      </c>
+      <c r="D103">
+        <v>544.31162424522574</v>
+      </c>
+      <c r="E103">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>174</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>3351.4339999999997</v>
+      </c>
+      <c r="D104">
+        <v>545.77341806988272</v>
+      </c>
+      <c r="E104">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>175</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>3370.2909999999997</v>
+      </c>
+      <c r="D105">
+        <v>547.29331684212741</v>
+      </c>
+      <c r="E105">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>176</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>3389.1479999999997</v>
+      </c>
+      <c r="D106">
+        <v>548.87425448125589</v>
+      </c>
+      <c r="E106">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>177</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>3408.0049999999997</v>
+      </c>
+      <c r="D107">
+        <v>550.51922148047709</v>
+      </c>
+      <c r="E107">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>178</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <v>3426.8619999999996</v>
+      </c>
+      <c r="D108">
+        <v>552.23126490691504</v>
+      </c>
+      <c r="E108">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>179</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <v>3445.7189999999996</v>
+      </c>
+      <c r="D109">
+        <v>554.01348840160529</v>
+      </c>
+      <c r="E109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>180</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <v>3464.5759999999996</v>
+      </c>
+      <c r="D110">
+        <v>555.86905217950255</v>
+      </c>
+      <c r="E110">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add right gear autos.
</commit_message>
<xml_diff>
--- a/conf/shooter_data.xlsx
+++ b/conf/shooter_data.xlsx
@@ -9,18 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="14300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -29,9 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Speed</t>
-  </si>
-  <si>
     <t>Distance</t>
   </si>
   <si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Elevation</t>
+  </si>
+  <si>
+    <t>Speed</t>
   </si>
   <si>
     <t>Hopper</t>
@@ -50,7 +53,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -58,7 +61,8 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -85,16 +89,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -123,7 +137,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -135,7 +149,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -152,9 +166,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -187,9 +201,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -369,1889 +383,2911 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:E170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:E110"/>
+      <selection activeCell="F1" sqref="F1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="8.83203125" style="3"/>
+    <col min="3" max="4" width="8.83203125" style="4"/>
+    <col min="5" max="5" width="8.83203125" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>72</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
         <v>1428.02</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>437.23645671509507</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>73</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
         <v>1446.877</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>437.93711585281255</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>74</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
         <v>1465.7339999999999</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>438.6909663204865</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>75</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
         <v>1484.5909999999999</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>439.49522807209462</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>76</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
         <v>1503.4480000000001</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>440.34717763552874</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>77</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
         <v>1522.3050000000001</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>441.24414811259408</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>78</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
         <v>1541.162</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>442.18352917901086</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>79</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
         <v>1560.019</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>443.16276708441217</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>80</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
         <v>1578.876</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4">
         <v>444.17936465234629</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>81</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
         <v>1597.7329999999999</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
         <v>445.23088128027496</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>82</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
         <v>1616.59</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
         <v>446.31493293957374</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>83</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
         <v>1635.4469999999999</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="4">
         <v>447.4291921755331</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>84</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
         <v>1654.3039999999999</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="4">
         <v>448.57138810735626</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>85</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
         <v>1673.1610000000001</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="4">
         <v>449.73930642816163</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>86</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
         <v>1692.018</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <v>450.93078940498094</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>87</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
         <v>1710.875</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="4">
         <v>452.14373587876048</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>88</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
         <v>1729.732</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="4">
         <v>453.37610126436027</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>89</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
         <v>1748.5889999999999</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="4">
         <v>454.62589755055444</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>90</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4">
         <v>1767.4459999999999</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="4">
         <v>455.89119330003086</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="3">
         <v>91</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
         <v>1786.3029999999999</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="4">
         <v>457.17011364939196</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="3">
         <v>92</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4">
         <v>1805.16</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="4">
         <v>458.46084030915415</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="3">
         <v>93</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2">
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4">
         <v>1824.0170000000001</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="4">
         <v>459.76161156374712</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="3">
         <v>94</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24" s="2">
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4">
         <v>1842.874</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="4">
         <v>461.07072227151582</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>95</v>
       </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25" s="2">
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4">
         <v>1861.731</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="4">
         <v>462.38652386471847</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="3">
         <v>96</v>
       </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26" s="2">
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="C26" s="4">
         <v>1880.588</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="4">
         <v>463.70742434952706</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="3">
         <v>97</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27" s="2">
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4">
         <v>1899.4449999999999</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="4">
         <v>465.03188830602869</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="3">
         <v>98</v>
       </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28" s="2">
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4">
         <v>1918.3019999999999</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="4">
         <v>466.35843688822308</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="3">
         <v>99</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="4">
         <v>1937.1589999999999</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="4">
         <v>467.6856478240253</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="3">
         <v>100</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30" s="2">
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+      <c r="C30" s="4">
         <v>1956.0159999999998</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="4">
         <v>469.01215541526369</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="3">
         <v>101</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31" s="2">
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4">
         <v>1974.873</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="4">
         <v>470.33665053768084</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="3">
         <v>102</v>
       </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32" s="2">
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+      <c r="C32" s="4">
         <v>1993.73</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="4">
         <v>471.65788064093329</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="3">
         <v>103</v>
       </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33" s="2">
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+      <c r="C33" s="4">
         <v>2012.587</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="4">
         <v>472.97464974859179</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="3">
         <v>104</v>
       </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34" s="2">
+      <c r="B34" s="3">
+        <v>0</v>
+      </c>
+      <c r="C34" s="4">
         <v>2031.444</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="4">
         <v>474.28581845814108</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="3">
         <v>105</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35" s="2">
+      <c r="B35" s="3">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4">
         <v>2050.3009999999999</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="4">
         <v>475.59030394098011</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="3">
         <v>106</v>
       </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36" s="2">
+      <c r="B36" s="3">
+        <v>0</v>
+      </c>
+      <c r="C36" s="4">
         <v>2069.1579999999999</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="4">
         <v>476.88707994242088</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="3">
         <v>107</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37" s="2">
+      <c r="B37" s="3">
+        <v>0</v>
+      </c>
+      <c r="C37" s="4">
         <v>2088.0149999999999</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="4">
         <v>478.17517678169077</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="3">
         <v>108</v>
       </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="C38" s="2">
+      <c r="B38" s="3">
+        <v>0</v>
+      </c>
+      <c r="C38" s="4">
         <v>2106.8719999999998</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="4">
         <v>479.45368135193064</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="3">
         <v>109</v>
       </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39" s="2">
+      <c r="B39" s="3">
+        <v>0</v>
+      </c>
+      <c r="C39" s="4">
         <v>2125.7289999999998</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="4">
         <v>480.7217371201956</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="3">
         <v>110</v>
       </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40" s="2">
+      <c r="B40" s="3">
+        <v>0</v>
+      </c>
+      <c r="C40" s="4">
         <v>2144.5859999999998</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="4">
         <v>481.97854412745403</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="3">
         <v>111</v>
       </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="C41" s="2">
+      <c r="B41" s="3">
+        <v>0</v>
+      </c>
+      <c r="C41" s="4">
         <v>2163.4429999999998</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="4">
         <v>483.22335898858944</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="A42" s="3">
         <v>112</v>
       </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42" s="2">
+      <c r="B42" s="3">
+        <v>0</v>
+      </c>
+      <c r="C42" s="4">
         <v>2182.2999999999997</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="4">
         <v>484.45549489239863</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="A43" s="3">
         <v>113</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43" s="2">
+      <c r="B43" s="3">
+        <v>0</v>
+      </c>
+      <c r="C43" s="4">
         <v>2201.1569999999997</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="4">
         <v>485.67432160159194</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="A44" s="3">
         <v>114</v>
       </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44" s="2">
+      <c r="B44" s="3">
+        <v>0</v>
+      </c>
+      <c r="C44" s="4">
         <v>2220.0139999999997</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="4">
         <v>486.87926545279595</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="A45" s="3">
         <v>115</v>
       </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="C45" s="2">
+      <c r="B45" s="3">
+        <v>0</v>
+      </c>
+      <c r="C45" s="4">
         <v>2238.8709999999996</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="4">
         <v>488.06980935654826</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
+      <c r="A46" s="3">
         <v>116</v>
       </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46" s="2">
+      <c r="B46" s="3">
+        <v>0</v>
+      </c>
+      <c r="C46" s="4">
         <v>2257.7279999999996</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="4">
         <v>489.24549279730365</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
+      <c r="A47" s="3">
         <v>117</v>
       </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47" s="2">
+      <c r="B47" s="3">
+        <v>0</v>
+      </c>
+      <c r="C47" s="4">
         <v>2276.5849999999996</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="4">
         <v>490.40591183342792</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48">
+      <c r="A48" s="3">
         <v>118</v>
       </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
-      <c r="C48" s="2">
+      <c r="B48" s="3">
+        <v>0</v>
+      </c>
+      <c r="C48" s="4">
         <v>2295.4419999999996</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="4">
         <v>491.55071909720243</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49">
+      <c r="A49" s="3">
         <v>119</v>
       </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49" s="2">
+      <c r="B49" s="3">
+        <v>0</v>
+      </c>
+      <c r="C49" s="4">
         <v>2314.2989999999995</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="4">
         <v>492.67962379482344</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50">
+      <c r="A50" s="3">
         <v>120</v>
       </c>
-      <c r="B50">
-        <v>0</v>
-      </c>
-      <c r="C50" s="2">
+      <c r="B50" s="3">
+        <v>0</v>
+      </c>
+      <c r="C50" s="4">
         <v>2333.1559999999999</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="4">
         <v>493.79239170639937</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51">
+      <c r="A51" s="3">
         <v>121</v>
       </c>
-      <c r="B51">
-        <v>0</v>
-      </c>
-      <c r="C51" s="2">
+      <c r="B51" s="3">
+        <v>0</v>
+      </c>
+      <c r="C51" s="4">
         <v>2352.0129999999999</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="4">
         <v>494.88884518595376</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52">
+      <c r="A52" s="3">
         <v>122</v>
       </c>
-      <c r="B52">
-        <v>0</v>
-      </c>
-      <c r="C52" s="2">
+      <c r="B52" s="3">
+        <v>0</v>
+      </c>
+      <c r="C52" s="4">
         <v>2370.87</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="4">
         <v>495.96886316142434</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53">
+      <c r="A53" s="3">
         <v>123</v>
       </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
-      <c r="C53" s="2">
+      <c r="B53" s="3">
+        <v>0</v>
+      </c>
+      <c r="C53" s="4">
         <v>2389.7269999999999</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="4">
         <v>497.03238113466193</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54">
+      <c r="A54" s="3">
         <v>124</v>
       </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
-      <c r="C54" s="2">
+      <c r="B54" s="3">
+        <v>0</v>
+      </c>
+      <c r="C54" s="4">
         <v>2408.5839999999998</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="4">
         <v>498.07939118143315</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55">
+      <c r="A55" s="3">
         <v>125</v>
       </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
-      <c r="C55" s="2">
+      <c r="B55" s="3">
+        <v>0</v>
+      </c>
+      <c r="C55" s="4">
         <v>2427.4409999999998</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="4">
         <v>499.10994195141632</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56">
+      <c r="A56" s="3">
         <v>126</v>
       </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
-      <c r="C56" s="2">
+      <c r="B56" s="3">
+        <v>0</v>
+      </c>
+      <c r="C56" s="4">
         <v>2446.2979999999998</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="4">
         <v>500.12413866820577</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57">
+      <c r="A57" s="3">
         <v>127</v>
       </c>
-      <c r="B57">
-        <v>0</v>
-      </c>
-      <c r="C57" s="2">
+      <c r="B57" s="3">
+        <v>0</v>
+      </c>
+      <c r="C57" s="4">
         <v>2465.1549999999997</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="4">
         <v>501.12214312930848</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58">
+      <c r="A58" s="3">
         <v>128</v>
       </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
-      <c r="C58" s="2">
+      <c r="B58" s="3">
+        <v>0</v>
+      </c>
+      <c r="C58" s="4">
         <v>2484.0119999999997</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="4">
         <v>502.1041737061463</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59">
+      <c r="A59" s="3">
         <v>129</v>
       </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
-      <c r="C59" s="2">
+      <c r="B59" s="3">
+        <v>0</v>
+      </c>
+      <c r="C59" s="4">
         <v>2502.8689999999997</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="4">
         <v>503.07050534405528</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60">
+      <c r="A60" s="3">
         <v>130</v>
       </c>
-      <c r="B60">
-        <v>0</v>
-      </c>
-      <c r="C60" s="2">
+      <c r="B60" s="3">
+        <v>0</v>
+      </c>
+      <c r="C60" s="4">
         <v>2521.7259999999997</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="4">
         <v>504.02146956228432</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61">
+      <c r="A61" s="3">
         <v>131</v>
       </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-      <c r="C61" s="2">
+      <c r="B61" s="3">
+        <v>0</v>
+      </c>
+      <c r="C61" s="4">
         <v>2540.5829999999996</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61" s="4">
         <v>504.95745445399837</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62">
+      <c r="A62" s="3">
         <v>132</v>
       </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
-      <c r="C62" s="2">
+      <c r="B62" s="3">
+        <v>0</v>
+      </c>
+      <c r="C62" s="4">
         <v>2559.4399999999996</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="4">
         <v>505.87890468627472</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63">
+      <c r="A63" s="3">
         <v>133</v>
       </c>
-      <c r="B63">
-        <v>0</v>
-      </c>
-      <c r="C63" s="2">
+      <c r="B63" s="3">
+        <v>0</v>
+      </c>
+      <c r="C63" s="4">
         <v>2578.2969999999996</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="4">
         <v>506.78632150010424</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64">
+      <c r="A64" s="3">
         <v>134</v>
       </c>
-      <c r="B64">
-        <v>0</v>
-      </c>
-      <c r="C64" s="2">
+      <c r="B64" s="3">
+        <v>0</v>
+      </c>
+      <c r="C64" s="4">
         <v>2597.1539999999995</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64" s="4">
         <v>507.68026271039378</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65">
+      <c r="A65" s="3">
         <v>135</v>
       </c>
-      <c r="B65">
-        <v>0</v>
-      </c>
-      <c r="C65" s="2">
+      <c r="B65" s="3">
+        <v>0</v>
+      </c>
+      <c r="C65" s="4">
         <v>2616.0109999999995</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65" s="4">
         <v>508.56134270596306</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66">
+      <c r="A66" s="3">
         <v>136</v>
       </c>
-      <c r="B66">
-        <v>0</v>
-      </c>
-      <c r="C66" s="2">
+      <c r="B66" s="3">
+        <v>0</v>
+      </c>
+      <c r="C66" s="4">
         <v>2634.8679999999995</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66" s="4">
         <v>509.43023244954577</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67">
+      <c r="A67" s="3">
         <v>137</v>
       </c>
-      <c r="B67">
-        <v>0</v>
-      </c>
-      <c r="C67" s="2">
+      <c r="B67" s="3">
+        <v>0</v>
+      </c>
+      <c r="C67" s="4">
         <v>2653.7249999999999</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67" s="4">
         <v>510.28765947779073</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68">
+      <c r="A68" s="3">
         <v>138</v>
       </c>
-      <c r="B68">
-        <v>0</v>
-      </c>
-      <c r="C68" s="2">
+      <c r="B68" s="3">
+        <v>0</v>
+      </c>
+      <c r="C68" s="4">
         <v>2672.5819999999999</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68" s="4">
         <v>511.1344079012589</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69">
+      <c r="A69" s="3">
         <v>139</v>
       </c>
-      <c r="B69">
-        <v>0</v>
-      </c>
-      <c r="C69" s="2">
+      <c r="B69" s="3">
+        <v>0</v>
+      </c>
+      <c r="C69" s="4">
         <v>2691.4389999999999</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D69" s="4">
         <v>511.97131840442705</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70">
+      <c r="A70" s="3">
         <v>140</v>
       </c>
-      <c r="B70">
-        <v>0</v>
-      </c>
-      <c r="C70" s="2">
+      <c r="B70" s="3">
+        <v>0</v>
+      </c>
+      <c r="C70" s="4">
         <v>2710.2959999999998</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D70" s="4">
         <v>512.79928824568435</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71">
+      <c r="A71" s="3">
         <v>141</v>
       </c>
-      <c r="B71">
-        <v>0</v>
-      </c>
-      <c r="C71" s="2">
+      <c r="B71" s="3">
+        <v>0</v>
+      </c>
+      <c r="C71" s="4">
         <v>2729.1529999999998</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71" s="4">
         <v>513.61927125733644</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72">
+      <c r="A72" s="3">
         <v>142</v>
       </c>
-      <c r="B72">
-        <v>0</v>
-      </c>
-      <c r="C72" s="2">
+      <c r="B72" s="3">
+        <v>0</v>
+      </c>
+      <c r="C72" s="4">
         <v>2748.0099999999998</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D72" s="4">
         <v>514.43227784559997</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73">
+      <c r="A73" s="3">
         <v>143</v>
       </c>
-      <c r="B73">
-        <v>0</v>
-      </c>
-      <c r="C73" s="2">
+      <c r="B73" s="3">
+        <v>0</v>
+      </c>
+      <c r="C73" s="4">
         <v>2766.8669999999997</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D73" s="4">
         <v>515.23937499060901</v>
       </c>
-      <c r="E73">
+      <c r="E73" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74">
+      <c r="A74" s="3">
         <v>144</v>
       </c>
-      <c r="B74">
-        <v>0</v>
-      </c>
-      <c r="C74" s="2">
+      <c r="B74" s="3">
+        <v>0</v>
+      </c>
+      <c r="C74" s="4">
         <v>2785.7239999999997</v>
       </c>
-      <c r="D74" s="2">
+      <c r="D74" s="4">
         <v>516.04168624640681</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75">
+      <c r="A75" s="3">
         <v>145</v>
       </c>
-      <c r="B75">
-        <v>0</v>
-      </c>
-      <c r="C75" s="2">
+      <c r="B75" s="3">
+        <v>0</v>
+      </c>
+      <c r="C75" s="4">
         <v>2804.5809999999997</v>
       </c>
-      <c r="D75" s="2">
+      <c r="D75" s="4">
         <v>516.84039174095608</v>
       </c>
-      <c r="E75">
+      <c r="E75" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76">
+      <c r="A76" s="3">
         <v>146</v>
       </c>
-      <c r="B76">
-        <v>0</v>
-      </c>
-      <c r="C76" s="2">
+      <c r="B76" s="3">
+        <v>0</v>
+      </c>
+      <c r="C76" s="4">
         <v>2823.4379999999996</v>
       </c>
-      <c r="D76" s="2">
+      <c r="D76" s="4">
         <v>517.6367281761319</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77">
+      <c r="A77" s="3">
         <v>147</v>
       </c>
-      <c r="B77">
-        <v>0</v>
-      </c>
-      <c r="C77" s="2">
+      <c r="B77" s="3">
+        <v>0</v>
+      </c>
+      <c r="C77" s="4">
         <v>2842.2949999999996</v>
       </c>
-      <c r="D77" s="2">
+      <c r="D77" s="4">
         <v>518.43198882772015</v>
       </c>
-      <c r="E77">
+      <c r="E77" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78">
+      <c r="A78" s="3">
         <v>148</v>
       </c>
-      <c r="B78">
-        <v>0</v>
-      </c>
-      <c r="C78" s="2">
+      <c r="B78" s="3">
+        <v>0</v>
+      </c>
+      <c r="C78" s="4">
         <v>2861.1519999999996</v>
       </c>
-      <c r="D78" s="2">
+      <c r="D78" s="4">
         <v>519.22752354542502</v>
       </c>
-      <c r="E78">
+      <c r="E78" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79">
+      <c r="A79" s="3">
         <v>149</v>
       </c>
-      <c r="B79">
-        <v>0</v>
-      </c>
-      <c r="C79" s="2">
+      <c r="B79" s="3">
+        <v>0</v>
+      </c>
+      <c r="C79" s="4">
         <v>2880.0089999999996</v>
       </c>
-      <c r="D79" s="2">
+      <c r="D79" s="4">
         <v>520.02473875286171</v>
       </c>
-      <c r="E79">
+      <c r="E79" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80">
+      <c r="A80" s="3">
         <v>150</v>
       </c>
-      <c r="B80">
-        <v>0</v>
-      </c>
-      <c r="C80" s="2">
+      <c r="B80" s="3">
+        <v>0</v>
+      </c>
+      <c r="C80" s="4">
         <v>2898.8659999999995</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D80" s="4">
         <v>520.82509744756146</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81">
+      <c r="A81" s="3">
         <v>151</v>
       </c>
-      <c r="B81">
-        <v>0</v>
-      </c>
-      <c r="C81" s="2">
+      <c r="B81" s="3">
+        <v>0</v>
+      </c>
+      <c r="C81" s="4">
         <v>2917.7229999999995</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D81" s="4">
         <v>521.63011920096835</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82">
+      <c r="A82" s="3">
         <v>152</v>
       </c>
-      <c r="B82">
-        <v>0</v>
-      </c>
-      <c r="C82" s="2">
+      <c r="B82" s="3">
+        <v>0</v>
+      </c>
+      <c r="C82" s="4">
         <v>2936.58</v>
       </c>
-      <c r="D82" s="2">
+      <c r="D82" s="4">
         <v>522.44138015844248</v>
       </c>
-      <c r="E82">
+      <c r="E82" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83">
+      <c r="A83" s="3">
         <v>153</v>
       </c>
-      <c r="B83">
-        <v>0</v>
-      </c>
-      <c r="C83" s="2">
+      <c r="B83" s="3">
+        <v>0</v>
+      </c>
+      <c r="C83" s="4">
         <v>2955.4369999999999</v>
       </c>
-      <c r="D83" s="2">
+      <c r="D83" s="4">
         <v>523.26051303925362</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84">
+      <c r="A84" s="3">
         <v>154</v>
       </c>
-      <c r="B84">
-        <v>0</v>
-      </c>
-      <c r="C84" s="2">
+      <c r="B84" s="3">
+        <v>0</v>
+      </c>
+      <c r="C84" s="4">
         <v>2974.2939999999999</v>
       </c>
-      <c r="D84" s="2">
+      <c r="D84" s="4">
         <v>524.08920713659074</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85">
+      <c r="A85" s="3">
         <v>155</v>
       </c>
-      <c r="B85">
-        <v>0</v>
-      </c>
-      <c r="C85" s="2">
+      <c r="B85" s="3">
+        <v>0</v>
+      </c>
+      <c r="C85" s="4">
         <v>2993.1509999999998</v>
       </c>
-      <c r="D85" s="2">
+      <c r="D85" s="4">
         <v>524.92920831755475</v>
       </c>
-      <c r="E85">
+      <c r="E85" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86">
+      <c r="A86" s="3">
         <v>156</v>
       </c>
-      <c r="B86">
-        <v>0</v>
-      </c>
-      <c r="C86" s="2">
+      <c r="B86" s="3">
+        <v>0</v>
+      </c>
+      <c r="C86" s="4">
         <v>3012.0079999999998</v>
       </c>
-      <c r="D86" s="2">
+      <c r="D86" s="4">
         <v>525.78231902315804</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87">
+      <c r="A87" s="3">
         <v>157</v>
       </c>
-      <c r="B87">
-        <v>0</v>
-      </c>
-      <c r="C87">
+      <c r="B87" s="3">
+        <v>0</v>
+      </c>
+      <c r="C87" s="4">
         <v>3030.8649999999998</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="4">
         <v>526.65039826833174</v>
       </c>
-      <c r="E87">
+      <c r="E87" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88">
+      <c r="A88" s="3">
         <v>158</v>
       </c>
-      <c r="B88">
-        <v>0</v>
-      </c>
-      <c r="C88">
+      <c r="B88" s="3">
+        <v>0</v>
+      </c>
+      <c r="C88" s="4">
         <v>3049.7219999999998</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="4">
         <v>527.53536164191667</v>
       </c>
-      <c r="E88">
+      <c r="E88" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89">
+      <c r="A89" s="3">
         <v>159</v>
       </c>
-      <c r="B89">
-        <v>0</v>
-      </c>
-      <c r="C89">
+      <c r="B89" s="3">
+        <v>0</v>
+      </c>
+      <c r="C89" s="4">
         <v>3068.5789999999997</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="4">
         <v>528.439181306671</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90">
+      <c r="A90" s="3">
         <v>160</v>
       </c>
-      <c r="B90">
-        <v>0</v>
-      </c>
-      <c r="C90">
+      <c r="B90" s="3">
+        <v>0</v>
+      </c>
+      <c r="C90" s="4">
         <v>3087.4359999999997</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="4">
         <v>529.36388599926488</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91">
+      <c r="A91" s="3">
         <v>161</v>
       </c>
-      <c r="B91">
-        <v>0</v>
-      </c>
-      <c r="C91">
+      <c r="B91" s="3">
+        <v>0</v>
+      </c>
+      <c r="C91" s="4">
         <v>3106.2929999999997</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="4">
         <v>530.31156103028582</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92">
+      <c r="A92" s="3">
         <v>162</v>
       </c>
-      <c r="B92">
-        <v>0</v>
-      </c>
-      <c r="C92">
+      <c r="B92" s="3">
+        <v>0</v>
+      </c>
+      <c r="C92" s="4">
         <v>3125.1499999999996</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="4">
         <v>531.2843482842278</v>
       </c>
-      <c r="E92">
+      <c r="E92" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93">
+      <c r="A93" s="3">
         <v>163</v>
       </c>
-      <c r="B93">
-        <v>0</v>
-      </c>
-      <c r="C93">
+      <c r="B93" s="3">
+        <v>0</v>
+      </c>
+      <c r="C93" s="4">
         <v>3144.0069999999996</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="4">
         <v>532.28444621950769</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94">
+      <c r="A94" s="3">
         <v>164</v>
       </c>
-      <c r="B94">
-        <v>0</v>
-      </c>
-      <c r="C94">
+      <c r="B94" s="3">
+        <v>0</v>
+      </c>
+      <c r="C94" s="4">
         <v>3162.8639999999996</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="4">
         <v>533.31410986845106</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95">
+      <c r="A95" s="3">
         <v>165</v>
       </c>
-      <c r="B95">
-        <v>0</v>
-      </c>
-      <c r="C95">
+      <c r="B95" s="3">
+        <v>0</v>
+      </c>
+      <c r="C95" s="4">
         <v>3181.7209999999995</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="4">
         <v>534.3756508373009</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96">
+      <c r="A96" s="3">
         <v>166</v>
       </c>
-      <c r="B96">
-        <v>0</v>
-      </c>
-      <c r="C96">
+      <c r="B96" s="3">
+        <v>0</v>
+      </c>
+      <c r="C96" s="4">
         <v>3200.5779999999995</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="4">
         <v>535.47143730620849</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97">
+      <c r="A97" s="3">
         <v>167</v>
       </c>
-      <c r="B97">
-        <v>0</v>
-      </c>
-      <c r="C97">
+      <c r="B97" s="3">
+        <v>0</v>
+      </c>
+      <c r="C97" s="4">
         <v>3219.4349999999995</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="4">
         <v>536.60389402924659</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98">
+      <c r="A98" s="3">
         <v>168</v>
       </c>
-      <c r="B98">
-        <v>0</v>
-      </c>
-      <c r="C98">
+      <c r="B98" s="3">
+        <v>0</v>
+      </c>
+      <c r="C98" s="4">
         <v>3238.2919999999995</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="4">
         <v>537.77550233439626</v>
       </c>
-      <c r="E98">
+      <c r="E98" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99">
+      <c r="A99" s="3">
         <v>169</v>
       </c>
-      <c r="B99">
-        <v>0</v>
-      </c>
-      <c r="C99">
+      <c r="B99" s="3">
+        <v>0</v>
+      </c>
+      <c r="C99" s="4">
         <v>3257.1489999999999</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="4">
         <v>538.98880012355596</v>
       </c>
-      <c r="E99">
+      <c r="E99" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100">
+      <c r="A100" s="3">
         <v>170</v>
       </c>
-      <c r="B100">
-        <v>0</v>
-      </c>
-      <c r="C100">
+      <c r="B100" s="3">
+        <v>0</v>
+      </c>
+      <c r="C100" s="4">
         <v>3276.0059999999999</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="4">
         <v>540.24638187253697</v>
       </c>
-      <c r="E100">
+      <c r="E100" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101">
+      <c r="A101" s="3">
         <v>171</v>
       </c>
-      <c r="B101">
-        <v>0</v>
-      </c>
-      <c r="C101">
+      <c r="B101" s="3">
+        <v>0</v>
+      </c>
+      <c r="C101" s="4">
         <v>3294.8629999999998</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="4">
         <v>541.55089863106252</v>
       </c>
-      <c r="E101">
+      <c r="E101" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102">
+      <c r="A102" s="3">
         <v>172</v>
       </c>
-      <c r="B102">
-        <v>0</v>
-      </c>
-      <c r="C102">
+      <c r="B102" s="3">
+        <v>0</v>
+      </c>
+      <c r="C102" s="4">
         <v>3313.72</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="4">
         <v>542.9050580227746</v>
       </c>
-      <c r="E102">
+      <c r="E102" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103">
+      <c r="A103" s="3">
         <v>173</v>
       </c>
-      <c r="B103">
-        <v>0</v>
-      </c>
-      <c r="C103">
+      <c r="B103" s="3">
+        <v>0</v>
+      </c>
+      <c r="C103" s="4">
         <v>3332.5769999999998</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="4">
         <v>544.31162424522574</v>
       </c>
-      <c r="E103">
+      <c r="E103" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104">
+      <c r="A104" s="3">
         <v>174</v>
       </c>
-      <c r="B104">
-        <v>0</v>
-      </c>
-      <c r="C104">
+      <c r="B104" s="3">
+        <v>0</v>
+      </c>
+      <c r="C104" s="4">
         <v>3351.4339999999997</v>
       </c>
-      <c r="D104">
+      <c r="D104" s="4">
         <v>545.77341806988272</v>
       </c>
-      <c r="E104">
+      <c r="E104" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105">
+      <c r="A105" s="3">
         <v>175</v>
       </c>
-      <c r="B105">
-        <v>0</v>
-      </c>
-      <c r="C105">
+      <c r="B105" s="3">
+        <v>0</v>
+      </c>
+      <c r="C105" s="4">
         <v>3370.2909999999997</v>
       </c>
-      <c r="D105">
+      <c r="D105" s="4">
         <v>547.29331684212741</v>
       </c>
-      <c r="E105">
+      <c r="E105" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106">
+      <c r="A106" s="3">
         <v>176</v>
       </c>
-      <c r="B106">
-        <v>0</v>
-      </c>
-      <c r="C106">
+      <c r="B106" s="3">
+        <v>0</v>
+      </c>
+      <c r="C106" s="4">
         <v>3389.1479999999997</v>
       </c>
-      <c r="D106">
+      <c r="D106" s="4">
         <v>548.87425448125589</v>
       </c>
-      <c r="E106">
+      <c r="E106" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107">
+      <c r="A107" s="3">
         <v>177</v>
       </c>
-      <c r="B107">
-        <v>0</v>
-      </c>
-      <c r="C107">
+      <c r="B107" s="3">
+        <v>0</v>
+      </c>
+      <c r="C107" s="4">
         <v>3408.0049999999997</v>
       </c>
-      <c r="D107">
+      <c r="D107" s="4">
         <v>550.51922148047709</v>
       </c>
-      <c r="E107">
+      <c r="E107" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108">
+      <c r="A108" s="3">
         <v>178</v>
       </c>
-      <c r="B108">
-        <v>0</v>
-      </c>
-      <c r="C108">
+      <c r="B108" s="3">
+        <v>0</v>
+      </c>
+      <c r="C108" s="4">
         <v>3426.8619999999996</v>
       </c>
-      <c r="D108">
+      <c r="D108" s="4">
         <v>552.23126490691504</v>
       </c>
-      <c r="E108">
+      <c r="E108" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A109">
+      <c r="A109" s="3">
         <v>179</v>
       </c>
-      <c r="B109">
-        <v>0</v>
-      </c>
-      <c r="C109">
+      <c r="B109" s="3">
+        <v>0</v>
+      </c>
+      <c r="C109" s="4">
         <v>3445.7189999999996</v>
       </c>
-      <c r="D109">
+      <c r="D109" s="4">
         <v>554.01348840160529</v>
       </c>
-      <c r="E109">
+      <c r="E109" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110">
+      <c r="A110" s="3">
         <v>180</v>
       </c>
-      <c r="B110">
-        <v>0</v>
-      </c>
-      <c r="C110">
+      <c r="B110" s="3">
+        <v>0</v>
+      </c>
+      <c r="C110" s="4">
         <v>3464.5759999999996</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="4">
         <v>555.86905217950255</v>
       </c>
-      <c r="E110">
+      <c r="E110" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="3">
+        <v>181</v>
+      </c>
+      <c r="B111" s="3">
+        <v>0</v>
+      </c>
+      <c r="C111" s="4">
+        <v>3483.4329999999995</v>
+      </c>
+      <c r="D111" s="4">
+        <v>557.80117302946985</v>
+      </c>
+      <c r="E111" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="3">
+        <v>182</v>
+      </c>
+      <c r="B112" s="3">
+        <v>0</v>
+      </c>
+      <c r="C112" s="4">
+        <v>3502.2899999999995</v>
+      </c>
+      <c r="D112" s="4">
+        <v>559.81312431428853</v>
+      </c>
+      <c r="E112" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="3">
+        <v>183</v>
+      </c>
+      <c r="B113" s="3">
+        <v>0</v>
+      </c>
+      <c r="C113" s="4">
+        <v>3521.1469999999995</v>
+      </c>
+      <c r="D113" s="4">
+        <v>561.90823597065275</v>
+      </c>
+      <c r="E113" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="3">
+        <v>184</v>
+      </c>
+      <c r="B114" s="3">
+        <v>0</v>
+      </c>
+      <c r="C114" s="4">
+        <v>3540.0039999999999</v>
+      </c>
+      <c r="D114" s="4">
+        <v>564.08989450916954</v>
+      </c>
+      <c r="E114" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="3">
+        <v>185</v>
+      </c>
+      <c r="B115" s="3">
+        <v>0</v>
+      </c>
+      <c r="C115" s="4">
+        <v>3558.8609999999999</v>
+      </c>
+      <c r="D115" s="4">
+        <v>566.36154301435965</v>
+      </c>
+      <c r="E115" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="3">
+        <v>186</v>
+      </c>
+      <c r="B116" s="3">
+        <v>0</v>
+      </c>
+      <c r="C116" s="4">
+        <v>3577.7179999999998</v>
+      </c>
+      <c r="D116" s="4">
+        <v>568.7266811446608</v>
+      </c>
+      <c r="E116" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" s="3">
+        <v>187</v>
+      </c>
+      <c r="B117" s="3">
+        <v>0</v>
+      </c>
+      <c r="C117" s="4">
+        <v>3596.5749999999998</v>
+      </c>
+      <c r="D117" s="4">
+        <v>571.18886513242171</v>
+      </c>
+      <c r="E117" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" s="3">
+        <v>188</v>
+      </c>
+      <c r="B118" s="3">
+        <v>0</v>
+      </c>
+      <c r="C118" s="4">
+        <v>3615.4319999999998</v>
+      </c>
+      <c r="D118" s="4">
+        <v>573.75170778390805</v>
+      </c>
+      <c r="E118" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" s="3">
+        <v>189</v>
+      </c>
+      <c r="B119" s="3">
+        <v>0</v>
+      </c>
+      <c r="C119" s="4">
+        <v>3634.2889999999998</v>
+      </c>
+      <c r="D119" s="4">
+        <v>576.41887847929559</v>
+      </c>
+      <c r="E119" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="3">
+        <v>190</v>
+      </c>
+      <c r="B120" s="3">
+        <v>0</v>
+      </c>
+      <c r="C120" s="4">
+        <v>3653.1459999999997</v>
+      </c>
+      <c r="D120" s="4">
+        <v>579.19410317267841</v>
+      </c>
+      <c r="E120" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="3">
+        <v>191</v>
+      </c>
+      <c r="B121" s="3">
+        <v>0</v>
+      </c>
+      <c r="C121" s="4">
+        <v>3672.0029999999997</v>
+      </c>
+      <c r="D121" s="4">
+        <v>582.08116439206071</v>
+      </c>
+      <c r="E121" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" s="3">
+        <v>192</v>
+      </c>
+      <c r="B122" s="3">
+        <v>0</v>
+      </c>
+      <c r="C122" s="4">
+        <v>3690.8599999999997</v>
+      </c>
+      <c r="D122" s="4">
+        <v>585.08390123936226</v>
+      </c>
+      <c r="E122" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" s="3">
+        <v>193</v>
+      </c>
+      <c r="B123" s="3">
+        <v>0</v>
+      </c>
+      <c r="C123" s="4">
+        <v>3709.7169999999996</v>
+      </c>
+      <c r="D123" s="4">
+        <v>588.20620939042112</v>
+      </c>
+      <c r="E123" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="3">
+        <v>194</v>
+      </c>
+      <c r="B124" s="3">
+        <v>0</v>
+      </c>
+      <c r="C124" s="4">
+        <v>3728.5739999999996</v>
+      </c>
+      <c r="D124" s="4">
+        <v>591.45204109498093</v>
+      </c>
+      <c r="E124" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" s="3">
+        <v>195</v>
+      </c>
+      <c r="B125" s="3">
+        <v>0</v>
+      </c>
+      <c r="C125" s="4">
+        <v>3747.4309999999996</v>
+      </c>
+      <c r="D125" s="4">
+        <v>594.82540517670543</v>
+      </c>
+      <c r="E125" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" s="3">
+        <v>196</v>
+      </c>
+      <c r="B126" s="3">
+        <v>0</v>
+      </c>
+      <c r="C126" s="4">
+        <v>3766.2879999999996</v>
+      </c>
+      <c r="D126" s="4">
+        <v>598.33036703317123</v>
+      </c>
+      <c r="E126" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="3">
+        <v>197</v>
+      </c>
+      <c r="B127" s="3">
+        <v>0</v>
+      </c>
+      <c r="C127" s="4">
+        <v>3785.1449999999995</v>
+      </c>
+      <c r="D127" s="4">
+        <v>601.9710486358714</v>
+      </c>
+      <c r="E127" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="3">
+        <v>198</v>
+      </c>
+      <c r="B128" s="3">
+        <v>0</v>
+      </c>
+      <c r="C128" s="4">
+        <v>3804.0019999999995</v>
+      </c>
+      <c r="D128" s="4">
+        <v>605.75162853020367</v>
+      </c>
+      <c r="E128" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" s="3">
+        <v>199</v>
+      </c>
+      <c r="B129" s="3">
+        <v>0</v>
+      </c>
+      <c r="C129" s="4">
+        <v>3822.8589999999995</v>
+      </c>
+      <c r="D129" s="4">
+        <v>609.67634183549319</v>
+      </c>
+      <c r="E129" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" s="3">
+        <v>200</v>
+      </c>
+      <c r="B130" s="3">
+        <v>0</v>
+      </c>
+      <c r="C130" s="4">
+        <v>3841.7159999999994</v>
+      </c>
+      <c r="D130" s="4">
+        <v>613.74948024496791</v>
+      </c>
+      <c r="E130" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" s="3">
+        <v>201</v>
+      </c>
+      <c r="B131" s="3">
+        <v>0</v>
+      </c>
+      <c r="C131" s="4">
+        <v>3860.5729999999999</v>
+      </c>
+      <c r="D131" s="4">
+        <v>617.9753920257773</v>
+      </c>
+      <c r="E131" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" s="3">
+        <v>202</v>
+      </c>
+      <c r="B132" s="3">
+        <v>0</v>
+      </c>
+      <c r="C132" s="4">
+        <v>3879.43</v>
+      </c>
+      <c r="D132" s="4">
+        <v>622.35848201897818</v>
+      </c>
+      <c r="E132" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" s="3">
+        <v>203</v>
+      </c>
+      <c r="B133" s="3">
+        <v>0</v>
+      </c>
+      <c r="C133" s="4">
+        <v>3898.2869999999998</v>
+      </c>
+      <c r="D133" s="4">
+        <v>626.90321163954889</v>
+      </c>
+      <c r="E133" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" s="3">
+        <v>204</v>
+      </c>
+      <c r="B134" s="3">
+        <v>0</v>
+      </c>
+      <c r="C134" s="4">
+        <v>3917.1439999999998</v>
+      </c>
+      <c r="D134" s="4">
+        <v>631.61409887637694</v>
+      </c>
+      <c r="E134" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" s="3">
+        <v>205</v>
+      </c>
+      <c r="B135" s="3">
+        <v>0</v>
+      </c>
+      <c r="C135" s="4">
+        <v>3936.0009999999997</v>
+      </c>
+      <c r="D135" s="4">
+        <v>636.49571829226363</v>
+      </c>
+      <c r="E135" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" s="3">
+        <v>206</v>
+      </c>
+      <c r="B136" s="3">
+        <v>0</v>
+      </c>
+      <c r="C136" s="4">
+        <v>3954.8579999999997</v>
+      </c>
+      <c r="D136" s="4">
+        <v>641.55270102392581</v>
+      </c>
+      <c r="E136" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" s="3">
+        <v>207</v>
+      </c>
+      <c r="B137" s="3">
+        <v>0</v>
+      </c>
+      <c r="C137" s="4">
+        <v>3973.7149999999997</v>
+      </c>
+      <c r="D137" s="4">
+        <v>646.78973478199589</v>
+      </c>
+      <c r="E137" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" s="3">
+        <v>208</v>
+      </c>
+      <c r="B138" s="3">
+        <v>0</v>
+      </c>
+      <c r="C138" s="4">
+        <v>3992.5719999999997</v>
+      </c>
+      <c r="D138" s="4">
+        <v>652.21156385101824</v>
+      </c>
+      <c r="E138" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" s="3">
+        <v>209</v>
+      </c>
+      <c r="B139" s="3">
+        <v>0</v>
+      </c>
+      <c r="C139" s="4">
+        <v>4011.4289999999996</v>
+      </c>
+      <c r="D139" s="4">
+        <v>657.82298908945097</v>
+      </c>
+      <c r="E139" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140" s="3">
+        <v>210</v>
+      </c>
+      <c r="B140" s="3">
+        <v>0</v>
+      </c>
+      <c r="C140" s="4">
+        <v>4030.2859999999996</v>
+      </c>
+      <c r="D140" s="4">
+        <v>663.62886792966685</v>
+      </c>
+      <c r="E140" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" s="3">
+        <v>211</v>
+      </c>
+      <c r="B141" s="3">
+        <v>0</v>
+      </c>
+      <c r="C141" s="4">
+        <v>4049.1429999999996</v>
+      </c>
+      <c r="D141" s="4">
+        <v>669.63411437795151</v>
+      </c>
+      <c r="E141" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" s="3">
+        <v>212</v>
+      </c>
+      <c r="B142" s="3">
+        <v>0</v>
+      </c>
+      <c r="C142" s="4">
+        <v>4067.9999999999995</v>
+      </c>
+      <c r="D142" s="4">
+        <v>675.84369901450793</v>
+      </c>
+      <c r="E142" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" s="3">
+        <v>213</v>
+      </c>
+      <c r="B143" s="3">
+        <v>0</v>
+      </c>
+      <c r="C143" s="4">
+        <v>4086.8569999999995</v>
+      </c>
+      <c r="D143" s="4">
+        <v>682.26264899345017</v>
+      </c>
+      <c r="E143" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" s="3">
+        <v>214</v>
+      </c>
+      <c r="B144" s="3">
+        <v>0</v>
+      </c>
+      <c r="C144" s="4">
+        <v>4105.7139999999999</v>
+      </c>
+      <c r="D144" s="4">
+        <v>688.89604804280646</v>
+      </c>
+      <c r="E144" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" s="3">
+        <v>215</v>
+      </c>
+      <c r="B145" s="3">
+        <v>0</v>
+      </c>
+      <c r="C145" s="4">
+        <v>4124.5709999999999</v>
+      </c>
+      <c r="D145" s="4">
+        <v>695.74903646452242</v>
+      </c>
+      <c r="E145" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" s="3">
+        <v>216</v>
+      </c>
+      <c r="B146" s="3">
+        <v>0</v>
+      </c>
+      <c r="C146" s="4">
+        <v>4143.4279999999999</v>
+      </c>
+      <c r="D146" s="4">
+        <v>702.82681113445062</v>
+      </c>
+      <c r="E146" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" s="3">
+        <v>217</v>
+      </c>
+      <c r="B147" s="3">
+        <v>0</v>
+      </c>
+      <c r="C147" s="4">
+        <v>4162.2849999999999</v>
+      </c>
+      <c r="D147" s="4">
+        <v>710.13462550236738</v>
+      </c>
+      <c r="E147" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" s="3">
+        <v>218</v>
+      </c>
+      <c r="B148" s="3">
+        <v>0</v>
+      </c>
+      <c r="C148" s="4">
+        <v>4181.1419999999998</v>
+      </c>
+      <c r="D148" s="4">
+        <v>717.67778959195459</v>
+      </c>
+      <c r="E148" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" s="3">
+        <v>219</v>
+      </c>
+      <c r="B149" s="3">
+        <v>0</v>
+      </c>
+      <c r="C149" s="4">
+        <v>4199.9989999999998</v>
+      </c>
+      <c r="D149" s="4">
+        <v>725.46167000081152</v>
+      </c>
+      <c r="E149" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" s="3">
+        <v>220</v>
+      </c>
+      <c r="B150" s="3">
+        <v>0</v>
+      </c>
+      <c r="C150" s="4">
+        <v>4218.8559999999998</v>
+      </c>
+      <c r="D150" s="4">
+        <v>733.49168990045121</v>
+      </c>
+      <c r="E150" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" s="3">
+        <v>221</v>
+      </c>
+      <c r="B151" s="3">
+        <v>0</v>
+      </c>
+      <c r="C151" s="4">
+        <v>4237.7129999999997</v>
+      </c>
+      <c r="D151" s="4">
+        <v>741.77332903630497</v>
+      </c>
+      <c r="E151" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" s="3">
+        <v>222</v>
+      </c>
+      <c r="B152" s="3">
+        <v>0</v>
+      </c>
+      <c r="C152" s="4">
+        <v>4256.57</v>
+      </c>
+      <c r="D152" s="4">
+        <v>750.3121237277079</v>
+      </c>
+      <c r="E152" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" s="3">
+        <v>223</v>
+      </c>
+      <c r="B153" s="3">
+        <v>0</v>
+      </c>
+      <c r="C153" s="4">
+        <v>4275.4269999999997</v>
+      </c>
+      <c r="D153" s="4">
+        <v>759.11366686791791</v>
+      </c>
+      <c r="E153" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" s="3">
+        <v>224</v>
+      </c>
+      <c r="B154" s="3">
+        <v>0</v>
+      </c>
+      <c r="C154" s="4">
+        <v>4294.2839999999997</v>
+      </c>
+      <c r="D154" s="4">
+        <v>768.1836079241067</v>
+      </c>
+      <c r="E154" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" s="3">
+        <v>225</v>
+      </c>
+      <c r="B155" s="3">
+        <v>0</v>
+      </c>
+      <c r="C155" s="4">
+        <v>4313.1409999999996</v>
+      </c>
+      <c r="D155" s="4">
+        <v>777.52765293735331</v>
+      </c>
+      <c r="E155" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" s="3">
+        <v>226</v>
+      </c>
+      <c r="B156" s="3">
+        <v>0</v>
+      </c>
+      <c r="C156" s="4">
+        <v>4331.9979999999996</v>
+      </c>
+      <c r="D156" s="4">
+        <v>787.15156452265694</v>
+      </c>
+      <c r="E156" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" s="3">
+        <v>227</v>
+      </c>
+      <c r="B157" s="3">
+        <v>0</v>
+      </c>
+      <c r="C157" s="4">
+        <v>4350.8549999999996</v>
+      </c>
+      <c r="D157" s="4">
+        <v>797.06116186893325</v>
+      </c>
+      <c r="E157" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" s="3">
+        <v>228</v>
+      </c>
+      <c r="B158" s="3">
+        <v>0</v>
+      </c>
+      <c r="C158" s="4">
+        <v>4369.7119999999995</v>
+      </c>
+      <c r="D158" s="4">
+        <v>807.26232073900258</v>
+      </c>
+      <c r="E158" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" s="3">
+        <v>229</v>
+      </c>
+      <c r="B159" s="3">
+        <v>0</v>
+      </c>
+      <c r="C159" s="4">
+        <v>4388.5689999999995</v>
+      </c>
+      <c r="D159" s="4">
+        <v>817.76097346960489</v>
+      </c>
+      <c r="E159" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" s="3">
+        <v>230</v>
+      </c>
+      <c r="B160" s="3">
+        <v>0</v>
+      </c>
+      <c r="C160" s="4">
+        <v>4407.4259999999995</v>
+      </c>
+      <c r="D160" s="4">
+        <v>828.56310897139485</v>
+      </c>
+      <c r="E160" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" s="3">
+        <v>231</v>
+      </c>
+      <c r="B161" s="3">
+        <v>0</v>
+      </c>
+      <c r="C161" s="4">
+        <v>4426.2829999999994</v>
+      </c>
+      <c r="D161" s="4">
+        <v>839.67477272894223</v>
+      </c>
+      <c r="E161" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" s="3">
+        <v>232</v>
+      </c>
+      <c r="B162" s="3">
+        <v>0</v>
+      </c>
+      <c r="C162" s="4">
+        <v>4445.1399999999994</v>
+      </c>
+      <c r="D162" s="4">
+        <v>851.1020668007269</v>
+      </c>
+      <c r="E162" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" s="3">
+        <v>233</v>
+      </c>
+      <c r="B163" s="3">
+        <v>0</v>
+      </c>
+      <c r="C163" s="4">
+        <v>4463.9969999999994</v>
+      </c>
+      <c r="D163" s="4">
+        <v>862.85114981913978</v>
+      </c>
+      <c r="E163" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164" s="3">
+        <v>234</v>
+      </c>
+      <c r="B164" s="3">
+        <v>0</v>
+      </c>
+      <c r="C164" s="4">
+        <v>4482.8539999999994</v>
+      </c>
+      <c r="D164" s="4">
+        <v>874.92823699050007</v>
+      </c>
+      <c r="E164" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" s="3">
+        <v>235</v>
+      </c>
+      <c r="B165" s="3">
+        <v>0</v>
+      </c>
+      <c r="C165" s="4">
+        <v>4501.7109999999993</v>
+      </c>
+      <c r="D165" s="4">
+        <v>887.33960009502346</v>
+      </c>
+      <c r="E165" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" s="3">
+        <v>236</v>
+      </c>
+      <c r="B166" s="3">
+        <v>0</v>
+      </c>
+      <c r="C166" s="4">
+        <v>4520.5679999999993</v>
+      </c>
+      <c r="D166" s="4">
+        <v>900.0915674868512</v>
+      </c>
+      <c r="E166" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" s="3">
+        <v>237</v>
+      </c>
+      <c r="B167" s="3">
+        <v>0</v>
+      </c>
+      <c r="C167" s="4">
+        <v>4539.4249999999993</v>
+      </c>
+      <c r="D167" s="4">
+        <v>913.19052409403832</v>
+      </c>
+      <c r="E167" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" s="3">
+        <v>238</v>
+      </c>
+      <c r="B168" s="3">
+        <v>0</v>
+      </c>
+      <c r="C168" s="4">
+        <v>4558.2819999999992</v>
+      </c>
+      <c r="D168" s="4">
+        <v>926.64291141854358</v>
+      </c>
+      <c r="E168" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169" s="3">
+        <v>239</v>
+      </c>
+      <c r="B169" s="3">
+        <v>0</v>
+      </c>
+      <c r="C169" s="4">
+        <v>4577.1389999999992</v>
+      </c>
+      <c r="D169" s="4">
+        <v>940.45522753625221</v>
+      </c>
+      <c r="E169" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" s="3">
+        <v>240</v>
+      </c>
+      <c r="B170" s="3">
+        <v>0</v>
+      </c>
+      <c r="C170" s="4">
+        <v>4595.9960000000001</v>
+      </c>
+      <c r="D170" s="4">
+        <v>954.63402709695595</v>
+      </c>
+      <c r="E170" s="3">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tweaks for state games.
</commit_message>
<xml_diff>
--- a/conf/shooter_data.xlsx
+++ b/conf/shooter_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="14300"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="14320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -383,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E170"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:L1048576"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -424,7 +424,7 @@
         <v>1428.02</v>
       </c>
       <c r="D2" s="4">
-        <v>437.23645671509507</v>
+        <v>440.27514384998631</v>
       </c>
       <c r="E2" s="3">
         <v>8</v>
@@ -441,7 +441,7 @@
         <v>1446.877</v>
       </c>
       <c r="D3" s="4">
-        <v>437.93711585281255</v>
+        <v>440.62782300435993</v>
       </c>
       <c r="E3" s="3">
         <v>8</v>
@@ -458,7 +458,7 @@
         <v>1465.7339999999999</v>
       </c>
       <c r="D4" s="4">
-        <v>438.6909663204865</v>
+        <v>441.02827356885882</v>
       </c>
       <c r="E4" s="3">
         <v>8</v>
@@ -475,7 +475,7 @@
         <v>1484.5909999999999</v>
       </c>
       <c r="D5" s="4">
-        <v>439.49522807209462</v>
+        <v>441.48299817210409</v>
       </c>
       <c r="E5" s="3">
         <v>8</v>
@@ -492,7 +492,7 @@
         <v>1503.4480000000001</v>
       </c>
       <c r="D6" s="4">
-        <v>440.34717763552874</v>
+        <v>441.99711144930097</v>
       </c>
       <c r="E6" s="3">
         <v>8</v>
@@ -509,7 +509,7 @@
         <v>1522.3050000000001</v>
       </c>
       <c r="D7" s="4">
-        <v>441.24414811259408</v>
+        <v>442.57445352221384</v>
       </c>
       <c r="E7" s="3">
         <v>8</v>
@@ -526,7 +526,7 @@
         <v>1541.162</v>
       </c>
       <c r="D8" s="4">
-        <v>442.18352917901086</v>
+        <v>443.21769866434897</v>
       </c>
       <c r="E8" s="3">
         <v>8</v>
@@ -543,7 +543,7 @@
         <v>1560.019</v>
       </c>
       <c r="D9" s="4">
-        <v>443.16276708441217</v>
+        <v>443.92845923987898</v>
       </c>
       <c r="E9" s="3">
         <v>8</v>
@@ -560,7 +560,7 @@
         <v>1578.876</v>
       </c>
       <c r="D10" s="4">
-        <v>444.17936465234629</v>
+        <v>444.70738500496645</v>
       </c>
       <c r="E10" s="3">
         <v>8</v>
@@ -577,7 +577,7 @@
         <v>1597.7329999999999</v>
       </c>
       <c r="D11" s="4">
-        <v>445.23088128027496</v>
+        <v>445.55425785993339</v>
       </c>
       <c r="E11" s="3">
         <v>8</v>
@@ -594,7 +594,7 @@
         <v>1616.59</v>
       </c>
       <c r="D12" s="4">
-        <v>446.31493293957374</v>
+        <v>446.46808214099929</v>
       </c>
       <c r="E12" s="3">
         <v>8</v>
@@ -611,7 +611,7 @@
         <v>1635.4469999999999</v>
       </c>
       <c r="D13" s="4">
-        <v>447.4291921755331</v>
+        <v>447.44717054000557</v>
       </c>
       <c r="E13" s="3">
         <v>8</v>
@@ -628,7 +628,7 @@
         <v>1654.3039999999999</v>
       </c>
       <c r="D14" s="4">
-        <v>448.57138810735626</v>
+        <v>448.48922574087464</v>
       </c>
       <c r="E14" s="3">
         <v>8</v>
@@ -645,7 +645,7 @@
         <v>1673.1610000000001</v>
       </c>
       <c r="D15" s="4">
-        <v>449.73930642816163</v>
+        <v>449.59141786130476</v>
       </c>
       <c r="E15" s="3">
         <v>8</v>
@@ -662,7 +662,7 @@
         <v>1692.018</v>
       </c>
       <c r="D16" s="4">
-        <v>450.93078940498094</v>
+        <v>450.75045778817275</v>
       </c>
       <c r="E16" s="3">
         <v>8</v>
@@ -679,7 +679,7 @@
         <v>1710.875</v>
       </c>
       <c r="D17" s="4">
-        <v>452.14373587876048</v>
+        <v>451.96266649545123</v>
       </c>
       <c r="E17" s="3">
         <v>8</v>
@@ -696,7 +696,7 @@
         <v>1729.732</v>
       </c>
       <c r="D18" s="4">
-        <v>453.37610126436027</v>
+        <v>453.22404043302868</v>
       </c>
       <c r="E18" s="3">
         <v>8</v>
@@ -713,7 +713,7 @@
         <v>1748.5889999999999</v>
       </c>
       <c r="D19" s="4">
-        <v>454.62589755055444</v>
+        <v>454.53031307500987</v>
       </c>
       <c r="E19" s="3">
         <v>8</v>
@@ -730,7 +730,7 @@
         <v>1767.4459999999999</v>
       </c>
       <c r="D20" s="4">
-        <v>455.89119330003086</v>
+        <v>455.8770127163798</v>
       </c>
       <c r="E20" s="3">
         <v>8</v>
@@ -747,7 +747,7 @@
         <v>1786.3029999999999</v>
       </c>
       <c r="D21" s="4">
-        <v>457.17011364939196</v>
+        <v>457.25951660599367</v>
       </c>
       <c r="E21" s="3">
         <v>8</v>
@@ -764,7 +764,7 @@
         <v>1805.16</v>
       </c>
       <c r="D22" s="4">
-        <v>458.46084030915415</v>
+        <v>458.67310150524554</v>
       </c>
       <c r="E22" s="3">
         <v>8</v>
@@ -781,7 +781,7 @@
         <v>1824.0170000000001</v>
       </c>
       <c r="D23" s="4">
-        <v>459.76161156374712</v>
+        <v>460.11299076028354</v>
       </c>
       <c r="E23" s="3">
         <v>8</v>
@@ -798,7 +798,7 @@
         <v>1842.874</v>
       </c>
       <c r="D24" s="4">
-        <v>461.07072227151582</v>
+        <v>461.57439797681855</v>
       </c>
       <c r="E24" s="3">
         <v>8</v>
@@ -815,7 +815,7 @@
         <v>1861.731</v>
       </c>
       <c r="D25" s="4">
-        <v>462.38652386471847</v>
+        <v>463.05256738591834</v>
       </c>
       <c r="E25" s="3">
         <v>8</v>
@@ -832,7 +832,7 @@
         <v>1880.588</v>
       </c>
       <c r="D26" s="4">
-        <v>463.70742434952706</v>
+        <v>464.54281098940828</v>
       </c>
       <c r="E26" s="3">
         <v>8</v>
@@ -849,7 +849,7 @@
         <v>1899.4449999999999</v>
       </c>
       <c r="D27" s="4">
-        <v>465.03188830602869</v>
+        <v>466.04054257343068</v>
       </c>
       <c r="E27" s="3">
         <v>8</v>
@@ -866,7 +866,7 @@
         <v>1918.3019999999999</v>
       </c>
       <c r="D28" s="4">
-        <v>466.35843688822308</v>
+        <v>467.54130867869662</v>
       </c>
       <c r="E28" s="3">
         <v>8</v>
@@ -883,7 +883,7 @@
         <v>1937.1589999999999</v>
       </c>
       <c r="D29" s="4">
-        <v>467.6856478240253</v>
+        <v>469.04081661616055</v>
       </c>
       <c r="E29" s="3">
         <v>8</v>
@@ -900,7 +900,7 @@
         <v>1956.0159999999998</v>
       </c>
       <c r="D30" s="4">
-        <v>469.01215541526369</v>
+        <v>470.53495961657154</v>
       </c>
       <c r="E30" s="3">
         <v>8</v>
@@ -917,7 +917,7 @@
         <v>1974.873</v>
       </c>
       <c r="D31" s="4">
-        <v>470.33665053768084</v>
+        <v>472.01983920236944</v>
       </c>
       <c r="E31" s="3">
         <v>8</v>
@@ -934,7 +934,7 @@
         <v>1993.73</v>
       </c>
       <c r="D32" s="4">
-        <v>471.65788064093329</v>
+        <v>473.49178487111476</v>
       </c>
       <c r="E32" s="3">
         <v>8</v>
@@ -951,7 +951,7 @@
         <v>2012.587</v>
       </c>
       <c r="D33" s="4">
-        <v>472.97464974859179</v>
+        <v>474.94737117773457</v>
       </c>
       <c r="E33" s="3">
         <v>8</v>
@@ -968,7 +968,7 @@
         <v>2031.444</v>
       </c>
       <c r="D34" s="4">
-        <v>474.28581845814108</v>
+        <v>476.38343230588634</v>
       </c>
       <c r="E34" s="3">
         <v>8</v>
@@ -985,7 +985,7 @@
         <v>2050.3009999999999</v>
       </c>
       <c r="D35" s="4">
-        <v>475.59030394098011</v>
+        <v>477.79707421544572</v>
       </c>
       <c r="E35" s="3">
         <v>8</v>
@@ -1002,7 +1002,7 @@
         <v>2069.1579999999999</v>
       </c>
       <c r="D36" s="4">
-        <v>476.88707994242088</v>
+        <v>479.18568445575056</v>
       </c>
       <c r="E36" s="3">
         <v>8</v>
@@ -1019,7 +1019,7 @@
         <v>2088.0149999999999</v>
       </c>
       <c r="D37" s="4">
-        <v>478.17517678169077</v>
+        <v>480.54693973269877</v>
       </c>
       <c r="E37" s="3">
         <v>8</v>
@@ -1036,7 +1036,7 @@
         <v>2106.8719999999998</v>
       </c>
       <c r="D38" s="4">
-        <v>479.45368135193064</v>
+        <v>481.87881131825543</v>
       </c>
       <c r="E38" s="3">
         <v>8</v>
@@ -1053,7 +1053,7 @@
         <v>2125.7289999999998</v>
       </c>
       <c r="D39" s="4">
-        <v>480.7217371201956</v>
+        <v>483.17956839119415</v>
       </c>
       <c r="E39" s="3">
         <v>8</v>
@@ -1070,7 +1070,7 @@
         <v>2144.5859999999998</v>
       </c>
       <c r="D40" s="4">
-        <v>481.97854412745403</v>
+        <v>484.44777939768665</v>
       </c>
       <c r="E40" s="3">
         <v>8</v>
@@ -1087,7 +1087,7 @@
         <v>2163.4429999999998</v>
       </c>
       <c r="D41" s="4">
-        <v>483.22335898858944</v>
+        <v>485.68231151964119</v>
       </c>
       <c r="E41" s="3">
         <v>8</v>
@@ -1104,7 +1104,7 @@
         <v>2182.2999999999997</v>
       </c>
       <c r="D42" s="4">
-        <v>484.45549489239863</v>
+        <v>486.8823283406191</v>
       </c>
       <c r="E42" s="3">
         <v>8</v>
@@ -1121,7 +1121,7 @@
         <v>2201.1569999999997</v>
       </c>
       <c r="D43" s="4">
-        <v>485.67432160159194</v>
+        <v>488.04728579644416</v>
       </c>
       <c r="E43" s="3">
         <v>8</v>
@@ -1138,7 +1138,7 @@
         <v>2220.0139999999997</v>
       </c>
       <c r="D44" s="4">
-        <v>486.87926545279595</v>
+        <v>489.17692650033405</v>
       </c>
       <c r="E44" s="3">
         <v>8</v>
@@ -1155,7 +1155,7 @@
         <v>2238.8709999999996</v>
       </c>
       <c r="D45" s="4">
-        <v>488.06980935654826</v>
+        <v>490.27127253045455</v>
       </c>
       <c r="E45" s="3">
         <v>8</v>
@@ -1172,7 +1172,7 @@
         <v>2257.7279999999996</v>
       </c>
       <c r="D46" s="4">
-        <v>489.24549279730365</v>
+        <v>491.33061676848865</v>
       </c>
       <c r="E46" s="3">
         <v>8</v>
@@ -1189,7 +1189,7 @@
         <v>2276.5849999999996</v>
       </c>
       <c r="D47" s="4">
-        <v>490.40591183342792</v>
+        <v>492.35551287815451</v>
       </c>
       <c r="E47" s="3">
         <v>8</v>
@@ -1206,7 +1206,7 @@
         <v>2295.4419999999996</v>
       </c>
       <c r="D48" s="4">
-        <v>491.55071909720243</v>
+        <v>493.34676401189336</v>
       </c>
       <c r="E48" s="3">
         <v>8</v>
@@ -1223,7 +1223,7 @@
         <v>2314.2989999999995</v>
       </c>
       <c r="D49" s="4">
-        <v>492.67962379482344</v>
+        <v>494.30541033462487</v>
       </c>
       <c r="E49" s="3">
         <v>8</v>
@@ -1240,7 +1240,7 @@
         <v>2333.1559999999999</v>
       </c>
       <c r="D50" s="4">
-        <v>493.79239170639937</v>
+        <v>495.23271545273292</v>
       </c>
       <c r="E50" s="3">
         <v>8</v>
@@ -1257,7 +1257,7 @@
         <v>2352.0129999999999</v>
       </c>
       <c r="D51" s="4">
-        <v>494.88884518595376</v>
+        <v>496.13015183715015</v>
       </c>
       <c r="E51" s="3">
         <v>8</v>
@@ -1274,7 +1274,7 @@
         <v>2370.87</v>
       </c>
       <c r="D52" s="4">
-        <v>495.96886316142434</v>
+        <v>496.99938532943179</v>
       </c>
       <c r="E52" s="3">
         <v>8</v>
@@ -1291,7 +1291,7 @@
         <v>2389.7269999999999</v>
       </c>
       <c r="D53" s="4">
-        <v>497.03238113466193</v>
+        <v>497.84225881863949</v>
       </c>
       <c r="E53" s="3">
         <v>8</v>
@@ -1308,7 +1308,7 @@
         <v>2408.5839999999998</v>
       </c>
       <c r="D54" s="4">
-        <v>498.07939118143315</v>
+        <v>498.66077517767826</v>
       </c>
       <c r="E54" s="3">
         <v>8</v>
@@ -1325,7 +1325,7 @@
         <v>2427.4409999999998</v>
       </c>
       <c r="D55" s="4">
-        <v>499.10994195141632</v>
+        <v>499.45707954938825</v>
       </c>
       <c r="E55" s="3">
         <v>8</v>
@@ -1342,7 +1342,7 @@
         <v>2446.2979999999998</v>
       </c>
       <c r="D56" s="4">
-        <v>500.12413866820577</v>
+        <v>500.23344106768036</v>
       </c>
       <c r="E56" s="3">
         <v>8</v>
@@ -1359,7 +1359,7 @@
         <v>2465.1549999999997</v>
       </c>
       <c r="D57" s="4">
-        <v>501.12214312930848</v>
+        <v>500.99223410566174</v>
       </c>
       <c r="E57" s="3">
         <v>8</v>
@@ -1376,7 +1376,7 @@
         <v>2484.0119999999997</v>
       </c>
       <c r="D58" s="4">
-        <v>502.1041737061463</v>
+        <v>501.73591913733526</v>
       </c>
       <c r="E58" s="3">
         <v>8</v>
@@ -1393,7 +1393,7 @@
         <v>2502.8689999999997</v>
       </c>
       <c r="D59" s="4">
-        <v>503.07050534405528</v>
+        <v>502.46702330170501</v>
       </c>
       <c r="E59" s="3">
         <v>8</v>
@@ -1410,7 +1410,7 @@
         <v>2521.7259999999997</v>
       </c>
       <c r="D60" s="4">
-        <v>504.02146956228432</v>
+        <v>503.18812075873848</v>
       </c>
       <c r="E60" s="3">
         <v>8</v>
@@ -1427,7 +1427,7 @@
         <v>2540.5829999999996</v>
       </c>
       <c r="D61" s="4">
-        <v>504.95745445399837</v>
+        <v>503.90181292460602</v>
       </c>
       <c r="E61" s="3">
         <v>8</v>
@@ -1444,7 +1444,7 @@
         <v>2559.4399999999996</v>
       </c>
       <c r="D62" s="4">
-        <v>505.87890468627472</v>
+        <v>504.61070867562648</v>
       </c>
       <c r="E62" s="3">
         <v>8</v>
@@ -1461,7 +1461,7 @@
         <v>2578.2969999999996</v>
       </c>
       <c r="D63" s="4">
-        <v>506.78632150010424</v>
+        <v>505.31740460920537</v>
       </c>
       <c r="E63" s="3">
         <v>8</v>
@@ -1478,7 +1478,7 @@
         <v>2597.1539999999995</v>
       </c>
       <c r="D64" s="4">
-        <v>507.68026271039378</v>
+        <v>506.02446545036491</v>
       </c>
       <c r="E64" s="3">
         <v>8</v>
@@ -1495,7 +1495,7 @@
         <v>2616.0109999999995</v>
       </c>
       <c r="D65" s="4">
-        <v>508.56134270596306</v>
+        <v>506.7344046920216</v>
       </c>
       <c r="E65" s="3">
         <v>8</v>
@@ -1512,7 +1512,7 @@
         <v>2634.8679999999995</v>
       </c>
       <c r="D66" s="4">
-        <v>509.43023244954577</v>
+        <v>507.4496655584835</v>
       </c>
       <c r="E66" s="3">
         <v>8</v>
@@ -1529,7 +1529,7 @@
         <v>2653.7249999999999</v>
       </c>
       <c r="D67" s="4">
-        <v>510.28765947779073</v>
+        <v>508.17260238022118</v>
       </c>
       <c r="E67" s="3">
         <v>8</v>
@@ -1546,7 +1546,7 @@
         <v>2672.5819999999999</v>
       </c>
       <c r="D68" s="4">
-        <v>511.1344079012589</v>
+        <v>508.90546246811846</v>
       </c>
       <c r="E68" s="3">
         <v>8</v>
@@ -1563,7 +1563,7 @@
         <v>2691.4389999999999</v>
       </c>
       <c r="D69" s="4">
-        <v>511.97131840442705</v>
+        <v>509.6503685766902</v>
       </c>
       <c r="E69" s="3">
         <v>8</v>
@@ -1580,7 +1580,7 @@
         <v>2710.2959999999998</v>
       </c>
       <c r="D70" s="4">
-        <v>512.79928824568435</v>
+        <v>510.40930204362212</v>
       </c>
       <c r="E70" s="3">
         <v>8</v>
@@ -1597,7 +1597,7 @@
         <v>2729.1529999999998</v>
       </c>
       <c r="D71" s="4">
-        <v>513.61927125733644</v>
+        <v>511.18408669597829</v>
       </c>
       <c r="E71" s="3">
         <v>8</v>
@@ -1614,7 +1614,7 @@
         <v>2748.0099999999998</v>
       </c>
       <c r="D72" s="4">
-        <v>514.43227784559997</v>
+        <v>511.97637360948556</v>
       </c>
       <c r="E72" s="3">
         <v>8</v>
@@ -1631,7 +1631,7 @@
         <v>2766.8669999999997</v>
       </c>
       <c r="D73" s="4">
-        <v>515.23937499060901</v>
+        <v>512.787626811677</v>
       </c>
       <c r="E73" s="3">
         <v>8</v>
@@ -1648,7 +1648,7 @@
         <v>2785.7239999999997</v>
       </c>
       <c r="D74" s="4">
-        <v>516.04168624640681</v>
+        <v>513.61911001505632</v>
       </c>
       <c r="E74" s="3">
         <v>8</v>
@@ -1665,7 +1665,7 @@
         <v>2804.5809999999997</v>
       </c>
       <c r="D75" s="4">
-        <v>516.84039174095608</v>
+        <v>514.47187447174929</v>
       </c>
       <c r="E75" s="3">
         <v>8</v>
@@ -1682,7 +1682,7 @@
         <v>2823.4379999999996</v>
       </c>
       <c r="D76" s="4">
-        <v>517.6367281761319</v>
+        <v>515.34674803546204</v>
       </c>
       <c r="E76" s="3">
         <v>8</v>
@@ -1699,7 +1699,7 @@
         <v>2842.2949999999996</v>
       </c>
       <c r="D77" s="4">
-        <v>518.43198882772015</v>
+        <v>516.24432552080816</v>
       </c>
       <c r="E77" s="3">
         <v>8</v>
@@ -1716,7 +1716,7 @@
         <v>2861.1519999999996</v>
       </c>
       <c r="D78" s="4">
-        <v>519.22752354542502</v>
+        <v>517.16496044892392</v>
       </c>
       <c r="E78" s="3">
         <v>8</v>
@@ -1733,7 +1733,7 @@
         <v>2880.0089999999996</v>
       </c>
       <c r="D79" s="4">
-        <v>520.02473875286171</v>
+        <v>518.1087582662467</v>
       </c>
       <c r="E79" s="3">
         <v>8</v>
@@ -1750,7 +1750,7 @@
         <v>2898.8659999999995</v>
       </c>
       <c r="D80" s="4">
-        <v>520.82509744756146</v>
+        <v>519.0755711271222</v>
       </c>
       <c r="E80" s="3">
         <v>8</v>
@@ -1767,7 +1767,7 @@
         <v>2917.7229999999995</v>
       </c>
       <c r="D81" s="4">
-        <v>521.63011920096835</v>
+        <v>520.0649943272756</v>
       </c>
       <c r="E81" s="3">
         <v>8</v>
@@ -1784,7 +1784,7 @@
         <v>2936.58</v>
       </c>
       <c r="D82" s="4">
-        <v>522.44138015844248</v>
+        <v>521.07636447725508</v>
       </c>
       <c r="E82" s="3">
         <v>8</v>
@@ -1801,7 +1801,7 @@
         <v>2955.4369999999999</v>
       </c>
       <c r="D83" s="4">
-        <v>523.26051303925362</v>
+        <v>522.10875950481113</v>
       </c>
       <c r="E83" s="3">
         <v>8</v>
@@ -1818,7 +1818,7 @@
         <v>2974.2939999999999</v>
       </c>
       <c r="D84" s="4">
-        <v>524.08920713659074</v>
+        <v>523.16100057359563</v>
       </c>
       <c r="E84" s="3">
         <v>8</v>
@@ -1835,7 +1835,7 @@
         <v>2993.1509999999998</v>
       </c>
       <c r="D85" s="4">
-        <v>524.92920831755475</v>
+        <v>524.23165600931225</v>
       </c>
       <c r="E85" s="3">
         <v>8</v>
@@ -1852,7 +1852,7 @@
         <v>3012.0079999999998</v>
       </c>
       <c r="D86" s="4">
-        <v>525.78231902315804</v>
+        <v>525.31904731693339</v>
       </c>
       <c r="E86" s="3">
         <v>8</v>
@@ -1869,7 +1869,7 @@
         <v>3030.8649999999998</v>
       </c>
       <c r="D87" s="4">
-        <v>526.65039826833174</v>
+        <v>526.42125738526647</v>
       </c>
       <c r="E87" s="3">
         <v>8</v>
@@ -1886,7 +1886,7 @@
         <v>3049.7219999999998</v>
       </c>
       <c r="D88" s="4">
-        <v>527.53536164191667</v>
+        <v>527.53614095857029</v>
       </c>
       <c r="E88" s="3">
         <v>8</v>
@@ -1903,7 +1903,7 @@
         <v>3068.5789999999997</v>
       </c>
       <c r="D89" s="4">
-        <v>528.439181306671</v>
+        <v>528.66133747119875</v>
       </c>
       <c r="E89" s="3">
         <v>8</v>
@@ -1920,7 +1920,7 @@
         <v>3087.4359999999997</v>
       </c>
       <c r="D90" s="4">
-        <v>529.36388599926488</v>
+        <v>529.79428632938198</v>
       </c>
       <c r="E90" s="3">
         <v>8</v>
@@ -1937,7 +1937,7 @@
         <v>3106.2929999999997</v>
       </c>
       <c r="D91" s="4">
-        <v>530.31156103028582</v>
+        <v>530.93224473091232</v>
       </c>
       <c r="E91" s="3">
         <v>8</v>
@@ -1954,7 +1954,7 @@
         <v>3125.1499999999996</v>
       </c>
       <c r="D92" s="4">
-        <v>531.2843482842278</v>
+        <v>532.07230810979945</v>
       </c>
       <c r="E92" s="3">
         <v>8</v>
@@ -1971,7 +1971,7 @@
         <v>3144.0069999999996</v>
       </c>
       <c r="D93" s="4">
-        <v>532.28444621950769</v>
+        <v>533.21143329629831</v>
       </c>
       <c r="E93" s="3">
         <v>8</v>
@@ -1988,7 +1988,7 @@
         <v>3162.8639999999996</v>
       </c>
       <c r="D94" s="4">
-        <v>533.31410986845106</v>
+        <v>534.34646447895193</v>
       </c>
       <c r="E94" s="3">
         <v>8</v>
@@ -2005,7 +2005,7 @@
         <v>3181.7209999999995</v>
       </c>
       <c r="D95" s="4">
-        <v>534.3756508373009</v>
+        <v>535.47416205867466</v>
       </c>
       <c r="E95" s="3">
         <v>8</v>
@@ -2022,7 +2022,7 @@
         <v>3200.5779999999995</v>
       </c>
       <c r="D96" s="4">
-        <v>535.47143730620849</v>
+        <v>536.59123448258015</v>
       </c>
       <c r="E96" s="3">
         <v>8</v>
@@ -2039,7 +2039,7 @@
         <v>3219.4349999999995</v>
       </c>
       <c r="D97" s="4">
-        <v>536.60389402924659</v>
+        <v>537.69437314648803</v>
       </c>
       <c r="E97" s="3">
         <v>8</v>
@@ -2056,7 +2056,7 @@
         <v>3238.2919999999995</v>
       </c>
       <c r="D98" s="4">
-        <v>537.77550233439626</v>
+        <v>538.780290455451</v>
       </c>
       <c r="E98" s="3">
         <v>8</v>
@@ -2073,7 +2073,7 @@
         <v>3257.1489999999999</v>
       </c>
       <c r="D99" s="4">
-        <v>538.98880012355596</v>
+        <v>539.8457611285221</v>
       </c>
       <c r="E99" s="3">
         <v>8</v>
@@ -2090,7 +2090,7 @@
         <v>3276.0059999999999</v>
       </c>
       <c r="D100" s="4">
-        <v>540.24638187253697</v>
+        <v>540.88766683915583</v>
       </c>
       <c r="E100" s="3">
         <v>8</v>
@@ -2107,7 +2107,7 @@
         <v>3294.8629999999998</v>
       </c>
       <c r="D101" s="4">
-        <v>541.55089863106252</v>
+        <v>541.90304427858337</v>
       </c>
       <c r="E101" s="3">
         <v>8</v>
@@ -2124,7 +2124,7 @@
         <v>3313.72</v>
       </c>
       <c r="D102" s="4">
-        <v>542.9050580227746</v>
+        <v>542.8891367293063</v>
       </c>
       <c r="E102" s="3">
         <v>8</v>
@@ -2141,7 +2141,7 @@
         <v>3332.5769999999998</v>
       </c>
       <c r="D103" s="4">
-        <v>544.31162424522574</v>
+        <v>543.84344924153538</v>
       </c>
       <c r="E103" s="3">
         <v>8</v>
@@ -2158,7 +2158,7 @@
         <v>3351.4339999999997</v>
       </c>
       <c r="D104" s="4">
-        <v>545.77341806988272</v>
+        <v>544.76380749487271</v>
       </c>
       <c r="E104" s="3">
         <v>8</v>
@@ -2175,7 +2175,7 @@
         <v>3370.2909999999997</v>
       </c>
       <c r="D105" s="4">
-        <v>547.29331684212741</v>
+        <v>545.64842043987574</v>
       </c>
       <c r="E105" s="3">
         <v>8</v>
@@ -2192,7 +2192,7 @@
         <v>3389.1479999999997</v>
       </c>
       <c r="D106" s="4">
-        <v>548.87425448125589</v>
+        <v>546.49594680383143</v>
       </c>
       <c r="E106" s="3">
         <v>8</v>
@@ -2209,7 +2209,7 @@
         <v>3408.0049999999997</v>
       </c>
       <c r="D107" s="4">
-        <v>550.51922148047709</v>
+        <v>547.30556555283238</v>
       </c>
       <c r="E107" s="3">
         <v>8</v>
@@ -2226,7 +2226,7 @@
         <v>3426.8619999999996</v>
       </c>
       <c r="D108" s="4">
-        <v>552.23126490691504</v>
+        <v>548.07705039452685</v>
       </c>
       <c r="E108" s="3">
         <v>8</v>
@@ -2243,7 +2243,7 @@
         <v>3445.7189999999996</v>
       </c>
       <c r="D109" s="4">
-        <v>554.01348840160529</v>
+        <v>548.81084841503161</v>
       </c>
       <c r="E109" s="3">
         <v>8</v>
@@ -2260,1029 +2260,9 @@
         <v>3464.5759999999996</v>
       </c>
       <c r="D110" s="4">
-        <v>555.86905217950255</v>
+        <v>549.50816293253138</v>
       </c>
       <c r="E110" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111" s="3">
-        <v>181</v>
-      </c>
-      <c r="B111" s="3">
-        <v>0</v>
-      </c>
-      <c r="C111" s="4">
-        <v>3483.4329999999995</v>
-      </c>
-      <c r="D111" s="4">
-        <v>557.80117302946985</v>
-      </c>
-      <c r="E111" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112" s="3">
-        <v>182</v>
-      </c>
-      <c r="B112" s="3">
-        <v>0</v>
-      </c>
-      <c r="C112" s="4">
-        <v>3502.2899999999995</v>
-      </c>
-      <c r="D112" s="4">
-        <v>559.81312431428853</v>
-      </c>
-      <c r="E112" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A113" s="3">
-        <v>183</v>
-      </c>
-      <c r="B113" s="3">
-        <v>0</v>
-      </c>
-      <c r="C113" s="4">
-        <v>3521.1469999999995</v>
-      </c>
-      <c r="D113" s="4">
-        <v>561.90823597065275</v>
-      </c>
-      <c r="E113" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A114" s="3">
-        <v>184</v>
-      </c>
-      <c r="B114" s="3">
-        <v>0</v>
-      </c>
-      <c r="C114" s="4">
-        <v>3540.0039999999999</v>
-      </c>
-      <c r="D114" s="4">
-        <v>564.08989450916954</v>
-      </c>
-      <c r="E114" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115" s="3">
-        <v>185</v>
-      </c>
-      <c r="B115" s="3">
-        <v>0</v>
-      </c>
-      <c r="C115" s="4">
-        <v>3558.8609999999999</v>
-      </c>
-      <c r="D115" s="4">
-        <v>566.36154301435965</v>
-      </c>
-      <c r="E115" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" s="3">
-        <v>186</v>
-      </c>
-      <c r="B116" s="3">
-        <v>0</v>
-      </c>
-      <c r="C116" s="4">
-        <v>3577.7179999999998</v>
-      </c>
-      <c r="D116" s="4">
-        <v>568.7266811446608</v>
-      </c>
-      <c r="E116" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117" s="3">
-        <v>187</v>
-      </c>
-      <c r="B117" s="3">
-        <v>0</v>
-      </c>
-      <c r="C117" s="4">
-        <v>3596.5749999999998</v>
-      </c>
-      <c r="D117" s="4">
-        <v>571.18886513242171</v>
-      </c>
-      <c r="E117" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118" s="3">
-        <v>188</v>
-      </c>
-      <c r="B118" s="3">
-        <v>0</v>
-      </c>
-      <c r="C118" s="4">
-        <v>3615.4319999999998</v>
-      </c>
-      <c r="D118" s="4">
-        <v>573.75170778390805</v>
-      </c>
-      <c r="E118" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119" s="3">
-        <v>189</v>
-      </c>
-      <c r="B119" s="3">
-        <v>0</v>
-      </c>
-      <c r="C119" s="4">
-        <v>3634.2889999999998</v>
-      </c>
-      <c r="D119" s="4">
-        <v>576.41887847929559</v>
-      </c>
-      <c r="E119" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120" s="3">
-        <v>190</v>
-      </c>
-      <c r="B120" s="3">
-        <v>0</v>
-      </c>
-      <c r="C120" s="4">
-        <v>3653.1459999999997</v>
-      </c>
-      <c r="D120" s="4">
-        <v>579.19410317267841</v>
-      </c>
-      <c r="E120" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A121" s="3">
-        <v>191</v>
-      </c>
-      <c r="B121" s="3">
-        <v>0</v>
-      </c>
-      <c r="C121" s="4">
-        <v>3672.0029999999997</v>
-      </c>
-      <c r="D121" s="4">
-        <v>582.08116439206071</v>
-      </c>
-      <c r="E121" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A122" s="3">
-        <v>192</v>
-      </c>
-      <c r="B122" s="3">
-        <v>0</v>
-      </c>
-      <c r="C122" s="4">
-        <v>3690.8599999999997</v>
-      </c>
-      <c r="D122" s="4">
-        <v>585.08390123936226</v>
-      </c>
-      <c r="E122" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123" s="3">
-        <v>193</v>
-      </c>
-      <c r="B123" s="3">
-        <v>0</v>
-      </c>
-      <c r="C123" s="4">
-        <v>3709.7169999999996</v>
-      </c>
-      <c r="D123" s="4">
-        <v>588.20620939042112</v>
-      </c>
-      <c r="E123" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A124" s="3">
-        <v>194</v>
-      </c>
-      <c r="B124" s="3">
-        <v>0</v>
-      </c>
-      <c r="C124" s="4">
-        <v>3728.5739999999996</v>
-      </c>
-      <c r="D124" s="4">
-        <v>591.45204109498093</v>
-      </c>
-      <c r="E124" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125" s="3">
-        <v>195</v>
-      </c>
-      <c r="B125" s="3">
-        <v>0</v>
-      </c>
-      <c r="C125" s="4">
-        <v>3747.4309999999996</v>
-      </c>
-      <c r="D125" s="4">
-        <v>594.82540517670543</v>
-      </c>
-      <c r="E125" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A126" s="3">
-        <v>196</v>
-      </c>
-      <c r="B126" s="3">
-        <v>0</v>
-      </c>
-      <c r="C126" s="4">
-        <v>3766.2879999999996</v>
-      </c>
-      <c r="D126" s="4">
-        <v>598.33036703317123</v>
-      </c>
-      <c r="E126" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127" s="3">
-        <v>197</v>
-      </c>
-      <c r="B127" s="3">
-        <v>0</v>
-      </c>
-      <c r="C127" s="4">
-        <v>3785.1449999999995</v>
-      </c>
-      <c r="D127" s="4">
-        <v>601.9710486358714</v>
-      </c>
-      <c r="E127" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128" s="3">
-        <v>198</v>
-      </c>
-      <c r="B128" s="3">
-        <v>0</v>
-      </c>
-      <c r="C128" s="4">
-        <v>3804.0019999999995</v>
-      </c>
-      <c r="D128" s="4">
-        <v>605.75162853020367</v>
-      </c>
-      <c r="E128" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A129" s="3">
-        <v>199</v>
-      </c>
-      <c r="B129" s="3">
-        <v>0</v>
-      </c>
-      <c r="C129" s="4">
-        <v>3822.8589999999995</v>
-      </c>
-      <c r="D129" s="4">
-        <v>609.67634183549319</v>
-      </c>
-      <c r="E129" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A130" s="3">
-        <v>200</v>
-      </c>
-      <c r="B130" s="3">
-        <v>0</v>
-      </c>
-      <c r="C130" s="4">
-        <v>3841.7159999999994</v>
-      </c>
-      <c r="D130" s="4">
-        <v>613.74948024496791</v>
-      </c>
-      <c r="E130" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A131" s="3">
-        <v>201</v>
-      </c>
-      <c r="B131" s="3">
-        <v>0</v>
-      </c>
-      <c r="C131" s="4">
-        <v>3860.5729999999999</v>
-      </c>
-      <c r="D131" s="4">
-        <v>617.9753920257773</v>
-      </c>
-      <c r="E131" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A132" s="3">
-        <v>202</v>
-      </c>
-      <c r="B132" s="3">
-        <v>0</v>
-      </c>
-      <c r="C132" s="4">
-        <v>3879.43</v>
-      </c>
-      <c r="D132" s="4">
-        <v>622.35848201897818</v>
-      </c>
-      <c r="E132" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A133" s="3">
-        <v>203</v>
-      </c>
-      <c r="B133" s="3">
-        <v>0</v>
-      </c>
-      <c r="C133" s="4">
-        <v>3898.2869999999998</v>
-      </c>
-      <c r="D133" s="4">
-        <v>626.90321163954889</v>
-      </c>
-      <c r="E133" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A134" s="3">
-        <v>204</v>
-      </c>
-      <c r="B134" s="3">
-        <v>0</v>
-      </c>
-      <c r="C134" s="4">
-        <v>3917.1439999999998</v>
-      </c>
-      <c r="D134" s="4">
-        <v>631.61409887637694</v>
-      </c>
-      <c r="E134" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A135" s="3">
-        <v>205</v>
-      </c>
-      <c r="B135" s="3">
-        <v>0</v>
-      </c>
-      <c r="C135" s="4">
-        <v>3936.0009999999997</v>
-      </c>
-      <c r="D135" s="4">
-        <v>636.49571829226363</v>
-      </c>
-      <c r="E135" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A136" s="3">
-        <v>206</v>
-      </c>
-      <c r="B136" s="3">
-        <v>0</v>
-      </c>
-      <c r="C136" s="4">
-        <v>3954.8579999999997</v>
-      </c>
-      <c r="D136" s="4">
-        <v>641.55270102392581</v>
-      </c>
-      <c r="E136" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A137" s="3">
-        <v>207</v>
-      </c>
-      <c r="B137" s="3">
-        <v>0</v>
-      </c>
-      <c r="C137" s="4">
-        <v>3973.7149999999997</v>
-      </c>
-      <c r="D137" s="4">
-        <v>646.78973478199589</v>
-      </c>
-      <c r="E137" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A138" s="3">
-        <v>208</v>
-      </c>
-      <c r="B138" s="3">
-        <v>0</v>
-      </c>
-      <c r="C138" s="4">
-        <v>3992.5719999999997</v>
-      </c>
-      <c r="D138" s="4">
-        <v>652.21156385101824</v>
-      </c>
-      <c r="E138" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A139" s="3">
-        <v>209</v>
-      </c>
-      <c r="B139" s="3">
-        <v>0</v>
-      </c>
-      <c r="C139" s="4">
-        <v>4011.4289999999996</v>
-      </c>
-      <c r="D139" s="4">
-        <v>657.82298908945097</v>
-      </c>
-      <c r="E139" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A140" s="3">
-        <v>210</v>
-      </c>
-      <c r="B140" s="3">
-        <v>0</v>
-      </c>
-      <c r="C140" s="4">
-        <v>4030.2859999999996</v>
-      </c>
-      <c r="D140" s="4">
-        <v>663.62886792966685</v>
-      </c>
-      <c r="E140" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A141" s="3">
-        <v>211</v>
-      </c>
-      <c r="B141" s="3">
-        <v>0</v>
-      </c>
-      <c r="C141" s="4">
-        <v>4049.1429999999996</v>
-      </c>
-      <c r="D141" s="4">
-        <v>669.63411437795151</v>
-      </c>
-      <c r="E141" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A142" s="3">
-        <v>212</v>
-      </c>
-      <c r="B142" s="3">
-        <v>0</v>
-      </c>
-      <c r="C142" s="4">
-        <v>4067.9999999999995</v>
-      </c>
-      <c r="D142" s="4">
-        <v>675.84369901450793</v>
-      </c>
-      <c r="E142" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A143" s="3">
-        <v>213</v>
-      </c>
-      <c r="B143" s="3">
-        <v>0</v>
-      </c>
-      <c r="C143" s="4">
-        <v>4086.8569999999995</v>
-      </c>
-      <c r="D143" s="4">
-        <v>682.26264899345017</v>
-      </c>
-      <c r="E143" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A144" s="3">
-        <v>214</v>
-      </c>
-      <c r="B144" s="3">
-        <v>0</v>
-      </c>
-      <c r="C144" s="4">
-        <v>4105.7139999999999</v>
-      </c>
-      <c r="D144" s="4">
-        <v>688.89604804280646</v>
-      </c>
-      <c r="E144" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A145" s="3">
-        <v>215</v>
-      </c>
-      <c r="B145" s="3">
-        <v>0</v>
-      </c>
-      <c r="C145" s="4">
-        <v>4124.5709999999999</v>
-      </c>
-      <c r="D145" s="4">
-        <v>695.74903646452242</v>
-      </c>
-      <c r="E145" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A146" s="3">
-        <v>216</v>
-      </c>
-      <c r="B146" s="3">
-        <v>0</v>
-      </c>
-      <c r="C146" s="4">
-        <v>4143.4279999999999</v>
-      </c>
-      <c r="D146" s="4">
-        <v>702.82681113445062</v>
-      </c>
-      <c r="E146" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147" s="3">
-        <v>217</v>
-      </c>
-      <c r="B147" s="3">
-        <v>0</v>
-      </c>
-      <c r="C147" s="4">
-        <v>4162.2849999999999</v>
-      </c>
-      <c r="D147" s="4">
-        <v>710.13462550236738</v>
-      </c>
-      <c r="E147" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A148" s="3">
-        <v>218</v>
-      </c>
-      <c r="B148" s="3">
-        <v>0</v>
-      </c>
-      <c r="C148" s="4">
-        <v>4181.1419999999998</v>
-      </c>
-      <c r="D148" s="4">
-        <v>717.67778959195459</v>
-      </c>
-      <c r="E148" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A149" s="3">
-        <v>219</v>
-      </c>
-      <c r="B149" s="3">
-        <v>0</v>
-      </c>
-      <c r="C149" s="4">
-        <v>4199.9989999999998</v>
-      </c>
-      <c r="D149" s="4">
-        <v>725.46167000081152</v>
-      </c>
-      <c r="E149" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A150" s="3">
-        <v>220</v>
-      </c>
-      <c r="B150" s="3">
-        <v>0</v>
-      </c>
-      <c r="C150" s="4">
-        <v>4218.8559999999998</v>
-      </c>
-      <c r="D150" s="4">
-        <v>733.49168990045121</v>
-      </c>
-      <c r="E150" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A151" s="3">
-        <v>221</v>
-      </c>
-      <c r="B151" s="3">
-        <v>0</v>
-      </c>
-      <c r="C151" s="4">
-        <v>4237.7129999999997</v>
-      </c>
-      <c r="D151" s="4">
-        <v>741.77332903630497</v>
-      </c>
-      <c r="E151" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152" s="3">
-        <v>222</v>
-      </c>
-      <c r="B152" s="3">
-        <v>0</v>
-      </c>
-      <c r="C152" s="4">
-        <v>4256.57</v>
-      </c>
-      <c r="D152" s="4">
-        <v>750.3121237277079</v>
-      </c>
-      <c r="E152" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A153" s="3">
-        <v>223</v>
-      </c>
-      <c r="B153" s="3">
-        <v>0</v>
-      </c>
-      <c r="C153" s="4">
-        <v>4275.4269999999997</v>
-      </c>
-      <c r="D153" s="4">
-        <v>759.11366686791791</v>
-      </c>
-      <c r="E153" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A154" s="3">
-        <v>224</v>
-      </c>
-      <c r="B154" s="3">
-        <v>0</v>
-      </c>
-      <c r="C154" s="4">
-        <v>4294.2839999999997</v>
-      </c>
-      <c r="D154" s="4">
-        <v>768.1836079241067</v>
-      </c>
-      <c r="E154" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A155" s="3">
-        <v>225</v>
-      </c>
-      <c r="B155" s="3">
-        <v>0</v>
-      </c>
-      <c r="C155" s="4">
-        <v>4313.1409999999996</v>
-      </c>
-      <c r="D155" s="4">
-        <v>777.52765293735331</v>
-      </c>
-      <c r="E155" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A156" s="3">
-        <v>226</v>
-      </c>
-      <c r="B156" s="3">
-        <v>0</v>
-      </c>
-      <c r="C156" s="4">
-        <v>4331.9979999999996</v>
-      </c>
-      <c r="D156" s="4">
-        <v>787.15156452265694</v>
-      </c>
-      <c r="E156" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A157" s="3">
-        <v>227</v>
-      </c>
-      <c r="B157" s="3">
-        <v>0</v>
-      </c>
-      <c r="C157" s="4">
-        <v>4350.8549999999996</v>
-      </c>
-      <c r="D157" s="4">
-        <v>797.06116186893325</v>
-      </c>
-      <c r="E157" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A158" s="3">
-        <v>228</v>
-      </c>
-      <c r="B158" s="3">
-        <v>0</v>
-      </c>
-      <c r="C158" s="4">
-        <v>4369.7119999999995</v>
-      </c>
-      <c r="D158" s="4">
-        <v>807.26232073900258</v>
-      </c>
-      <c r="E158" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A159" s="3">
-        <v>229</v>
-      </c>
-      <c r="B159" s="3">
-        <v>0</v>
-      </c>
-      <c r="C159" s="4">
-        <v>4388.5689999999995</v>
-      </c>
-      <c r="D159" s="4">
-        <v>817.76097346960489</v>
-      </c>
-      <c r="E159" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A160" s="3">
-        <v>230</v>
-      </c>
-      <c r="B160" s="3">
-        <v>0</v>
-      </c>
-      <c r="C160" s="4">
-        <v>4407.4259999999995</v>
-      </c>
-      <c r="D160" s="4">
-        <v>828.56310897139485</v>
-      </c>
-      <c r="E160" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A161" s="3">
-        <v>231</v>
-      </c>
-      <c r="B161" s="3">
-        <v>0</v>
-      </c>
-      <c r="C161" s="4">
-        <v>4426.2829999999994</v>
-      </c>
-      <c r="D161" s="4">
-        <v>839.67477272894223</v>
-      </c>
-      <c r="E161" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A162" s="3">
-        <v>232</v>
-      </c>
-      <c r="B162" s="3">
-        <v>0</v>
-      </c>
-      <c r="C162" s="4">
-        <v>4445.1399999999994</v>
-      </c>
-      <c r="D162" s="4">
-        <v>851.1020668007269</v>
-      </c>
-      <c r="E162" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A163" s="3">
-        <v>233</v>
-      </c>
-      <c r="B163" s="3">
-        <v>0</v>
-      </c>
-      <c r="C163" s="4">
-        <v>4463.9969999999994</v>
-      </c>
-      <c r="D163" s="4">
-        <v>862.85114981913978</v>
-      </c>
-      <c r="E163" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A164" s="3">
-        <v>234</v>
-      </c>
-      <c r="B164" s="3">
-        <v>0</v>
-      </c>
-      <c r="C164" s="4">
-        <v>4482.8539999999994</v>
-      </c>
-      <c r="D164" s="4">
-        <v>874.92823699050007</v>
-      </c>
-      <c r="E164" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A165" s="3">
-        <v>235</v>
-      </c>
-      <c r="B165" s="3">
-        <v>0</v>
-      </c>
-      <c r="C165" s="4">
-        <v>4501.7109999999993</v>
-      </c>
-      <c r="D165" s="4">
-        <v>887.33960009502346</v>
-      </c>
-      <c r="E165" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A166" s="3">
-        <v>236</v>
-      </c>
-      <c r="B166" s="3">
-        <v>0</v>
-      </c>
-      <c r="C166" s="4">
-        <v>4520.5679999999993</v>
-      </c>
-      <c r="D166" s="4">
-        <v>900.0915674868512</v>
-      </c>
-      <c r="E166" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A167" s="3">
-        <v>237</v>
-      </c>
-      <c r="B167" s="3">
-        <v>0</v>
-      </c>
-      <c r="C167" s="4">
-        <v>4539.4249999999993</v>
-      </c>
-      <c r="D167" s="4">
-        <v>913.19052409403832</v>
-      </c>
-      <c r="E167" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A168" s="3">
-        <v>238</v>
-      </c>
-      <c r="B168" s="3">
-        <v>0</v>
-      </c>
-      <c r="C168" s="4">
-        <v>4558.2819999999992</v>
-      </c>
-      <c r="D168" s="4">
-        <v>926.64291141854358</v>
-      </c>
-      <c r="E168" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A169" s="3">
-        <v>239</v>
-      </c>
-      <c r="B169" s="3">
-        <v>0</v>
-      </c>
-      <c r="C169" s="4">
-        <v>4577.1389999999992</v>
-      </c>
-      <c r="D169" s="4">
-        <v>940.45522753625221</v>
-      </c>
-      <c r="E169" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A170" s="3">
-        <v>240</v>
-      </c>
-      <c r="B170" s="3">
-        <v>0</v>
-      </c>
-      <c r="C170" s="4">
-        <v>4595.9960000000001</v>
-      </c>
-      <c r="D170" s="4">
-        <v>954.63402709695595</v>
-      </c>
-      <c r="E170" s="3">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add boiler camera azimuth and range corrections
</commit_message>
<xml_diff>
--- a/conf/shooter_data.xlsx
+++ b/conf/shooter_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Distance</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Hopper</t>
+  </si>
+  <si>
+    <t>IN Delta</t>
   </si>
 </sst>
 </file>
@@ -89,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -101,6 +104,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -383,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -396,7 +405,7 @@
     <col min="5" max="5" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -412,8 +421,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>72</v>
       </c>
@@ -429,8 +441,11 @@
       <c r="E2" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="6">
+        <v>0.30267915437361809</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>73</v>
       </c>
@@ -446,8 +461,11 @@
       <c r="E3" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="6">
+        <v>0.35267915437361808</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>74</v>
       </c>
@@ -463,8 +481,11 @@
       <c r="E4" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="6">
+        <v>0.40045056449889671</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>75</v>
       </c>
@@ -480,8 +501,11 @@
       <c r="E5" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="6">
+        <v>0.45472460324526764</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>76</v>
       </c>
@@ -497,8 +521,11 @@
       <c r="E6" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="6">
+        <v>0.51411327719688416</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>77</v>
       </c>
@@ -514,8 +541,11 @@
       <c r="E7" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="6">
+        <v>0.57734207291287021</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>78</v>
       </c>
@@ -531,8 +561,11 @@
       <c r="E8" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="6">
+        <v>0.64324514213512884</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>79</v>
       </c>
@@ -548,8 +581,11 @@
       <c r="E9" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="6">
+        <v>0.71076057553000282</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>80</v>
       </c>
@@ -565,8 +601,11 @@
       <c r="E10" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="6">
+        <v>0.77892576508747879</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>81</v>
       </c>
@@ -582,8 +621,11 @@
       <c r="E11" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="6">
+        <v>0.84687285496693221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>82</v>
       </c>
@@ -599,8 +641,11 @@
       <c r="E12" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="6">
+        <v>0.91382428106589941</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>83</v>
       </c>
@@ -616,8 +661,11 @@
       <c r="E13" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="6">
+        <v>0.97908839900628664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>84</v>
       </c>
@@ -633,8 +681,11 @@
       <c r="E14" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="6">
+        <v>1.042055200869072</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>85</v>
       </c>
@@ -650,8 +701,11 @@
       <c r="E15" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="6">
+        <v>1.1021921204301179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>86</v>
       </c>
@@ -667,8 +721,11 @@
       <c r="E16" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="6">
+        <v>1.1590399268679903</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>87</v>
       </c>
@@ -684,8 +741,11 @@
       <c r="E17" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="6">
+        <v>1.212208707278478</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>88</v>
       </c>
@@ -701,8 +761,11 @@
       <c r="E18" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="6">
+        <v>1.2613739375774458</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>89</v>
       </c>
@@ -718,8 +781,11 @@
       <c r="E19" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="6">
+        <v>1.3062726419811952</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>90</v>
       </c>
@@ -735,8 +801,11 @@
       <c r="E20" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="6">
+        <v>1.3466996413699235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>91</v>
       </c>
@@ -752,8 +821,11 @@
       <c r="E21" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="6">
+        <v>1.3825038896138722</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>92</v>
       </c>
@@ -769,8 +841,11 @@
       <c r="E22" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="6">
+        <v>1.4135848992518731</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>93</v>
       </c>
@@ -786,8 +861,11 @@
       <c r="E23" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="6">
+        <v>1.4398892550379969</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>94</v>
       </c>
@@ -803,8 +881,11 @@
       <c r="E24" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="6">
+        <v>1.461407216535008</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>95</v>
       </c>
@@ -820,8 +901,11 @@
       <c r="E25" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="6">
+        <v>1.4781694090997917</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>96</v>
       </c>
@@ -837,8 +921,11 @@
       <c r="E26" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="6">
+        <v>1.4902436034899438</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>97</v>
       </c>
@@ -854,8 +941,11 @@
       <c r="E27" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="6">
+        <v>1.4977315840224037</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>98</v>
       </c>
@@ -871,8 +961,11 @@
       <c r="E28" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="6">
+        <v>1.5007661052659387</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>99</v>
       </c>
@@ -888,8 +981,11 @@
       <c r="E29" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="6">
+        <v>1.4995079374639317</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>100</v>
       </c>
@@ -905,8 +1001,11 @@
       <c r="E30" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="6">
+        <v>1.4941430004109861</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>101</v>
       </c>
@@ -922,8 +1021,11 @@
       <c r="E31" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="6">
+        <v>1.4848795857978985</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>102</v>
       </c>
@@ -939,8 +1041,11 @@
       <c r="E32" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="6">
+        <v>1.4719456687453203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>103</v>
       </c>
@@ -956,8 +1061,11 @@
       <c r="E33" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="6">
+        <v>1.4555863066198071</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>104</v>
       </c>
@@ -973,8 +1081,11 @@
       <c r="E34" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="6">
+        <v>1.4360611281517777</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>105</v>
       </c>
@@ -990,8 +1101,11 @@
       <c r="E35" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="6">
+        <v>1.4136419095593737</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>106</v>
       </c>
@@ -1007,8 +1121,11 @@
       <c r="E36" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="6">
+        <v>1.3886102403048426</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>107</v>
       </c>
@@ -1024,8 +1141,11 @@
       <c r="E37" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="6">
+        <v>1.3612552769482136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>108</v>
       </c>
@@ -1041,8 +1161,11 @@
       <c r="E38" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="6">
+        <v>1.3318715855566552</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>109</v>
       </c>
@@ -1058,8 +1181,11 @@
       <c r="E39" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="6">
+        <v>1.3007570729387226</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>110</v>
       </c>
@@ -1075,8 +1201,11 @@
       <c r="E40" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="6">
+        <v>1.2682110064924927</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>111</v>
       </c>
@@ -1092,8 +1221,11 @@
       <c r="E41" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="6">
+        <v>1.234532121954544</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>112</v>
       </c>
@@ -1109,8 +1241,11 @@
       <c r="E42" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="6">
+        <v>1.2000168209779076</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>113</v>
       </c>
@@ -1126,8 +1261,11 @@
       <c r="E43" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="6">
+        <v>1.1649574558250606</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>114</v>
       </c>
@@ -1143,8 +1281,11 @@
       <c r="E44" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="6">
+        <v>1.1296407038898906</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>115</v>
       </c>
@@ -1160,8 +1301,11 @@
       <c r="E45" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="6">
+        <v>1.094346030120505</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>116</v>
       </c>
@@ -1177,8 +1321,11 @@
       <c r="E46" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="6">
+        <v>1.0593442380341003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>117</v>
       </c>
@@ -1194,8 +1341,11 @@
       <c r="E47" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="6">
+        <v>1.0248961096658604</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>118</v>
       </c>
@@ -1211,8 +1361,11 @@
       <c r="E48" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="6">
+        <v>0.99125113373884233</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>119</v>
       </c>
@@ -1228,8 +1381,11 @@
       <c r="E49" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="6">
+        <v>0.95864632273151074</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>120</v>
       </c>
@@ -1245,8 +1401,11 @@
       <c r="E50" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="6">
+        <v>0.92730511810805183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>121</v>
       </c>
@@ -1262,8 +1421,11 @@
       <c r="E51" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="6">
+        <v>0.89743638441723306</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>122</v>
       </c>
@@ -1279,8 +1441,11 @@
       <c r="E52" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="6">
+        <v>0.86923349228163715</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>123</v>
       </c>
@@ -1296,8 +1461,11 @@
       <c r="E53" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="6">
+        <v>0.84287348920770455</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>124</v>
       </c>
@@ -1313,8 +1481,11 @@
       <c r="E54" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="6">
+        <v>0.8185163590387674</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>125</v>
       </c>
@@ -1330,8 +1501,11 @@
       <c r="E55" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="6">
+        <v>0.79630437170999357</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>126</v>
       </c>
@@ -1347,8 +1521,11 @@
       <c r="E56" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="6">
+        <v>0.77636151829210576</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>127</v>
       </c>
@@ -1364,8 +1541,11 @@
       <c r="E57" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="6">
+        <v>0.75879303798137698</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>128</v>
       </c>
@@ -1381,8 +1561,11 @@
       <c r="E58" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="6">
+        <v>0.74368503167352173</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>129</v>
       </c>
@@ -1398,8 +1581,11 @@
       <c r="E59" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" s="6">
+        <v>0.73110416436975356</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>130</v>
       </c>
@@ -1415,8 +1601,11 @@
       <c r="E60" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="6">
+        <v>0.72109745703346562</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>131</v>
       </c>
@@ -1432,8 +1621,11 @@
       <c r="E61" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="6">
+        <v>0.71369216586754192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>132</v>
       </c>
@@ -1449,8 +1641,11 @@
       <c r="E62" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="6">
+        <v>0.70889575102046365</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>133</v>
       </c>
@@ -1466,8 +1661,11 @@
       <c r="E63" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="6">
+        <v>0.70669593357888516</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>134</v>
       </c>
@@ -1483,8 +1681,11 @@
       <c r="E64" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" s="6">
+        <v>0.70706084115954582</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>135</v>
       </c>
@@ -1500,8 +1701,11 @@
       <c r="E65" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="6">
+        <v>0.70993924165668432</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>136</v>
       </c>
@@ -1517,8 +1721,11 @@
       <c r="E66" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" s="6">
+        <v>0.71526086646190379</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>137</v>
       </c>
@@ -1534,8 +1741,11 @@
       <c r="E67" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" s="6">
+        <v>0.72293682173767593</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>138</v>
       </c>
@@ -1551,8 +1761,11 @@
       <c r="E68" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" s="6">
+        <v>0.7328600878972793</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>139</v>
       </c>
@@ -1568,8 +1781,11 @@
       <c r="E69" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" s="6">
+        <v>0.74490610857174033</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>140</v>
       </c>
@@ -1585,8 +1801,11 @@
       <c r="E70" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="6">
+        <v>0.75893346693192143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>141</v>
       </c>
@@ -1602,8 +1821,11 @@
       <c r="E71" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" s="6">
+        <v>0.77478465235617477</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>142</v>
       </c>
@@ -1619,8 +1841,11 @@
       <c r="E72" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" s="6">
+        <v>0.79228691350726876</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>143</v>
       </c>
@@ -1636,8 +1861,11 @@
       <c r="E73" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" s="6">
+        <v>0.81125320219143759</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>144</v>
       </c>
@@ -1653,8 +1881,11 @@
       <c r="E74" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" s="6">
+        <v>0.83148320337932091</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>145</v>
       </c>
@@ -1670,8 +1901,11 @@
       <c r="E75" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" s="6">
+        <v>0.85276445669296663</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>146</v>
       </c>
@@ -1687,8 +1921,11 @@
       <c r="E76" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76" s="6">
+        <v>0.87487356371275382</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>147</v>
       </c>
@@ -1704,8 +1941,11 @@
       <c r="E77" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77" s="6">
+        <v>0.89757748534611892</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>148</v>
       </c>
@@ -1721,8 +1961,11 @@
       <c r="E78" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78" s="6">
+        <v>0.92063492811575998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>149</v>
       </c>
@@ -1738,8 +1981,11 @@
       <c r="E79" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79" s="6">
+        <v>0.94379781732277479</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>150</v>
       </c>
@@ -1755,8 +2001,11 @@
       <c r="E80" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80" s="6">
+        <v>0.96681286087550689</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>151</v>
       </c>
@@ -1772,8 +2021,11 @@
       <c r="E81" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81" s="6">
+        <v>0.98942320015339646</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>152</v>
       </c>
@@ -1789,8 +2041,11 @@
       <c r="E82" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82" s="6">
+        <v>1.0113701499794843</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>153</v>
       </c>
@@ -1806,8 +2061,11 @@
       <c r="E83" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83" s="6">
+        <v>1.0323950275560492</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>154</v>
       </c>
@@ -1823,8 +2081,11 @@
       <c r="E84" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84" s="6">
+        <v>1.0522410687844967</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>155</v>
       </c>
@@ -1840,8 +2101,11 @@
       <c r="E85" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85" s="6">
+        <v>1.0706554357166169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>156</v>
       </c>
@@ -1857,8 +2121,11 @@
       <c r="E86" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86" s="6">
+        <v>1.0873913076211466</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>157</v>
       </c>
@@ -1874,8 +2141,11 @@
       <c r="E87" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87" s="6">
+        <v>1.1022100683330791</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>158</v>
       </c>
@@ -1891,8 +2161,11 @@
       <c r="E88" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88" s="6">
+        <v>1.114883573303814</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>159</v>
       </c>
@@ -1908,8 +2181,11 @@
       <c r="E89" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89" s="6">
+        <v>1.1251965126284631</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>160</v>
       </c>
@@ -1925,8 +2201,11 @@
       <c r="E90" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90" s="6">
+        <v>1.1329488581832265</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>161</v>
       </c>
@@ -1942,8 +2221,11 @@
       <c r="E91" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91" s="6">
+        <v>1.1379584015303408</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>162</v>
       </c>
@@ -1959,8 +2241,11 @@
       <c r="E92" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92" s="6">
+        <v>1.1400633788871346</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>163</v>
       </c>
@@ -1976,8 +2261,11 @@
       <c r="E93" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93" s="6">
+        <v>1.139125186498859</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>164</v>
       </c>
@@ -1993,8 +2281,11 @@
       <c r="E94" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94" s="6">
+        <v>1.1350311826536199</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>165</v>
       </c>
@@ -2010,8 +2301,11 @@
       <c r="E95" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95" s="6">
+        <v>1.1276975797227351</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>166</v>
       </c>
@@ -2027,8 +2321,11 @@
       <c r="E96" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96" s="6">
+        <v>1.1170724239054834</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>167</v>
       </c>
@@ -2044,8 +2341,11 @@
       <c r="E97" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97" s="6">
+        <v>1.1031386639078846</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>168</v>
       </c>
@@ -2061,8 +2361,11 @@
       <c r="E98" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98" s="6">
+        <v>1.0859173089629621</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>169</v>
       </c>
@@ -2078,8 +2381,11 @@
       <c r="E99" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99" s="6">
+        <v>1.0654706730711041</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>170</v>
       </c>
@@ -2095,8 +2401,11 @@
       <c r="E100" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100" s="6">
+        <v>1.0419057106337277</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>171</v>
       </c>
@@ -2112,8 +2421,11 @@
       <c r="E101" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101" s="6">
+        <v>1.0153774394275388</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>172</v>
       </c>
@@ -2129,8 +2441,11 @@
       <c r="E102" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102" s="6">
+        <v>0.98609245072293561</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>173</v>
       </c>
@@ -2146,8 +2461,11 @@
       <c r="E103" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103" s="6">
+        <v>0.95431251222908031</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>174</v>
       </c>
@@ -2163,8 +2481,11 @@
       <c r="E104" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104" s="6">
+        <v>0.92035825333732646</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>175</v>
       </c>
@@ -2180,8 +2501,11 @@
       <c r="E105" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105" s="6">
+        <v>0.88461294500302756</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>176</v>
       </c>
@@ -2197,8 +2521,11 @@
       <c r="E106" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106" s="6">
+        <v>0.84752636395569425</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>177</v>
       </c>
@@ -2214,8 +2541,11 @@
       <c r="E107" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107" s="6">
+        <v>0.80961874900094699</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>178</v>
       </c>
@@ -2231,8 +2561,11 @@
       <c r="E108" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108" s="6">
+        <v>0.77148484169447329</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>179</v>
       </c>
@@ -2248,8 +2581,11 @@
       <c r="E109" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109" s="6">
+        <v>0.73379802050476428</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>180</v>
       </c>
@@ -2264,6 +2600,9 @@
       </c>
       <c r="E110" s="3">
         <v>8</v>
+      </c>
+      <c r="F110" s="6">
+        <v>0.69731451749976259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>